<commit_message>
refactor: ctfidf model and count vectorizer to replace the original tfidf vectorizer
</commit_message>
<xml_diff>
--- a/repo/article_topic.xlsx
+++ b/repo/article_topic.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B177"/>
+  <dimension ref="A1:B186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,7 +447,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -457,7 +457,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -467,7 +467,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -477,7 +477,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -497,7 +497,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -507,7 +507,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -517,7 +517,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -527,7 +527,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -537,7 +537,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -547,7 +547,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -557,7 +557,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -567,7 +567,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -577,7 +577,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -587,7 +587,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -597,7 +597,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -607,7 +607,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -617,7 +617,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -627,7 +627,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -637,7 +637,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -647,7 +647,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -657,7 +657,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -667,7 +667,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -677,7 +677,7 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -687,157 +687,157 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve">〔 記者 蔡亞樺 ／ 台北 報導 〕 台北市 信義區 出現 天坑   台北市 消防局 下午 3 時 13 分接 獲通報   信義區 崇德 街 60 巷 22 號前 新建 工地 旁 道路 地層下陷   長 15 公尺   寬 3 公尺   深度 2 至 3 公尺     附近 住家 門口 2 部機車 一部 腳踏車 瞬間 掉 進 天坑   幸無人 受傷     台北市 政府 表示   目前 已 疏散 鄰近 住戶   並劃 設 警戒 線   消防局 已先 成立 現場 指揮 站   建管處   新工處   道管 中心   瓦斯 公司   北水處 已 派員 趕 赴 現場 處理   信義區 長 已 趕 抵 現場 坐鎮 指揮   目前 評估 約 10 餘位 住戶 需要 安置     台北市 建築 管理 處 表示   該案 因連續 壁施作   已 派員至 現場 了解 處理 中   目前 了解 是 連續 壁 滲水   工地 正在 止水 當中   消防局 現場 協助 鄰 房民眾 疏散  </t>
+          <t>台北市 出現 天坑   今天下午 15 時許   台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   坑洞 長 15 公尺   寬 3 公尺   深度 2 到 3 公尺   目視 可 看到 機車   自行 車 陷落 坑中   同時 坑洞 波及 一旁 民宅 地基   目前 台北市 消防局 已經 疏散 鄰近 住戶 10 多人   並劃 設緊 戒線   並 通知 市府 相關 單位 到場 處理       天坑 位 於 新建 工地 民宅 中間 巷弄 道路   塌陷 時 發出 聲響   驚動 住戶   但 因為 坑洞 擋 在家 門前   第一 時間 無法 脫困   消防局 緊急 到場   以 爬梯 方式 救援 住戶 出來                             消防局 救出 2 名 女子   疏散 1 男 1 女   人員 已 全數 疏散 完畢   另外 1 名 85 歲 老婦   因長 期行動 不便   雖無外傷   意識 清醒   但家屬 要求 預防性 送醫   由 消防局 送北醫   由 於 天坑 危及 安全   影響 周遭 至少 五戶 民宅   部分 住戶 無法 回家   估計 10 餘人受 影響   將由 台北市 府 處理 安置 問題       台北市 信義區 出現 天坑   目前 市府 新工處   建管處   勞檢處 等 相關 單位 都 已 派 人 到場   現場 設置 指揮 所   初步 懷疑 與 民宅 對面 新建 工地 工程 有關   現以 灌漿 方式 緊急 處置   至於 天坑 出現 原因   將 交由 市府 建管   新工 等 單位 調查   台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>-1</v>
+        <v>13</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve">台北市 信義區 崇德 街今   13   日 下午 3 點 13 分   傳出 一處 新建 案 工地 旁 道路   地層下陷     馬 路上 出現 一個 長 15 公尺   寬 3 公尺   深度 約 4 公尺 天坑   摩托 車   腳踏車 都 掉入 坑洞   一旁 住戶 家門口 更是 危險   懸空     而 台北 市長 蔣萬安 稍早 前往 現場 勘查   受訪 時 表示   第一 時間 就 即刻 派員前 來   相關 單位 了 緊急 疏散   強調   當這次 事件 緊急 處置 告一段落 之 後   會 台北市 相關 工地 全面 清查   了解 是否 有類 似 這次 地面 坍塌 原因   積極 相關 處置   目前 對廠 商及 建築師 各 開罰 9 萬元   工地 勒令停工   蔣萬安 表示   初步 了解   聽 了 相關 單位 說明   我們 下午 3 點 13 分   消防局 接收 到 地方 反應 這邊 地層下陷   第一 時間 就 即刻 派員前 來   趕快 連絡 了 警察局   新工處   建管處   區 公所   自來 水處   瓦斯 公司   台電 等 相關 單位   了 緊急 疏散   蔣萬安 指出   跟 指揮官   相關 單位 來 說明   第一   人員 安全 最 重要   所以 相關 緊急 應變 處置 必須 盡速 完成   包括 疏散   安置 等等   將這次 地面 坍塌 可能 造成 損害 降到 最低   第二   就 旁邊 工地   目前 了解 可能 是 連續 壁 滲水 問題   已經 趕快 了 處理   盡速 找出 坍塌 原因   然後盡 快 排除   避免 坍塌 面積 持續 擴大   第三   會 就 這次 地面 坍塌 事件 進行 調查   當然 包括 工地 實施者   營造 商過 去 相關 紀錄   第四   當這次 事件 緊急 處置 告一段落 之 後   要 台北市 相關 工地 全面 清查   了解 是否 有類 似 這次 地面 坍塌 原因   要積 極來 相關 處置   蔣萬安 表示     我們 現在 已經 非常 努力 緊急 應變   處置   第一 時間 盡快 疏散 了 住戶   我 想 市民 朋友 安全 是 最 重要   目前 還在 緊急 處置   我 想 必要 話 我們 還是 希望 預防性 疏散     而 台北市 土木 技師 公會 理事 長 莊均緯 指出   還要 再 把 崩塌 孔洞 填補 完成   現在 還在 灌水 當中   水頭 差會 慢慢 達到 平衡   而 因 地質 條件屬 於 沙 跟 水   因此 擔心 擋 土 設施 破洞   只要 衝破 連續 壁 洞   勢必 擋 土 牆後面 會 崩塌   目前 要 把 崩塌 部分 用 混 泥土 灌足外   開 挖面 水平衡   只要 水 與 地下水位 一 平衡   土沙 部分 就 會靜止   就 不會 往開 挖面 流動   防止 二次 下陷   目前 搶救 可控 範圍   莊均緯 表示   通常 會 發生 這狀況   是 地面 本來 就 下陷   只是 下陷 又 再 造成 第二 崩塌   灌漿 部分 還是 從 最 底下 往上 灌   表層 部分 基本上 還是 有些 鬆 動   需要 等 水位 平衡 後   才能 達到 搶災 最終 停止 狀態   估計 應該 都 要 到 凌晨  </t>
+          <t>台北市 信義區 一處 新建 大樓 工地 旁 巷道   蹋陷   緊急 灌漿 回填   住戶 驚慌 撤離         消防局 於 15 時 13 分獲報   信義區 崇德 街 60 巷 22 號前 新建 工地 旁 道路 地層下陷 ( 長 15 公尺   寬 3 公尺   深度 2   3 公尺 )   幸無人 受傷                             警消 緊急 疏散 鄰近 住戶   並劃 設 警戒 線   消防局 已先 成立 現場 指揮 站   建管處   新工處   道管 中心   瓦斯 公司   北水處 已 派員 趕 赴 現場 處理   目前 評估 約 10 餘位 住戶 需要 安置   台北市 信義區 一處 新建 大樓 工地 旁 巷道 突然 塌陷   施工 單位 緊急 灌漿 回填   防止 塌陷 區域 擴大     記者 林俊良 ／ 攝影警 消緊 急 疏散 鄰近 住戶   並劃 設 警戒 線   消防局 已先 成立 現場 指揮 站   目前 評估 約 10 餘位 住戶 需要 安置   記者 林俊良 ／ 攝影 消防局 於 15 時 13 分獲報   信義區 崇德 街 60 巷 22 號前 新建 工地 旁 道路 地層下陷   警消 緊急 疏散 鄰近 住戶   並劃 設 警戒 線   消防局 已先 成立 現場 指揮 站   建管處   新工處   道管 中心   瓦斯 公司   北水處 已 派員 趕 赴 現場 處理   記者 林俊良 ／ 攝影 今天下午 台北市 信義區 一處 新建 大樓 工地 旁 巷道   突然 塌陷   住戶 心有 餘悸 驚慌 撤離   到 一旁 安全 區域   記者 林俊良 ／ 攝影 今天下午 台北市 信義區 一處 新建 大樓 工地 旁 巷道   突然 塌陷   警方 疏導 住戶 驚慌 撤離   目前 評估 約 10 餘位 住戶 需要 安置   記者 林俊良 ／ 攝影 台北市 信義區 一處 新建 大樓 工地 旁 巷道 突然 塌陷   施工 單位 緊急 灌漿 回填   防止 塌陷 區域 擴大     記者 林俊良 ／ 攝影</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve">【 17   27 ｜ 更新 天坑 初步 原因 】 信義區 崇德 街今   13   天 下午 3 點 13 分   傳出 一處 新建 案 工地 旁 道路   地層下陷     消防局 獲報 緊急 疏散 鄰近 住戶   無人 受傷   根據 消防局 獲報 消息   信義區 崇德 街 60 巷 22 號前 新建 工地 旁   出現 道路 地層下陷   馬 路上 出現 一個 長 15 公尺   寬 3 公尺   深度 約 4 公尺 天坑   摩托 車   腳踏車 都 掉入 坑洞   一旁 住戶 家門口 更是 危險   懸空     警消 人員 疏散 鄰近 住戶   所幸 無人 受傷   目前 劃設 警戒 線   建管處   新工處   道管 中心   瓦斯 公司   北水處 派員 趕 赴 現場 處理   信義區 區長 已 趕 抵 現場 坐鎮 指揮   目前 評估 約 10 餘位 住戶 需要 安置   這個 天坑 幾乎 占據 整條 巷弄   北市 建管處 初步 了解   由 於 住 戶 旁 就是 工地 施工   疑似 因為 工地 連續 壁施作   且 出現 滲水 狀況   才 釀成 天坑 出現   稍早 水泥 車緊 急先 進行 灌漿 作業   主要 基本 填補 坑洞   受影響 住戶 透露   剛剛 一度 5 名住 戶 受困 屋子 裡   所幸 消防 員協助 救援   而 三戶 門口 前端 地基 被 掏空   住戶 非常 擔心 房屋 可能 會 倒塌   地基 到底 穩不穩固   住 裡面 到底 安 不 安全   今天 晚上 到底 要 住 哪裡 等 問題   不過 關於後續 賠償 等 都 還要 進 一步 釐 清  </t>
+          <t>台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   台北 市長 蔣萬安 晚上 到場 關心並 指出   整個 狀況 控制 住 以 後   會針 對 台北市 工地   全面 清查   是不是 這次 事件 類 似的 情況   再積 極處理       蔣萬安 表示   工地 部分   市府 馬 上 勒令停工   找出 這次 地面 坍塌 原因   盡快 排除   避免 坍塌 面積 持續 擴大   這次 地層下陷 事件   整起 事件 會 完整 調查   並且 就 工地 全面 檢視   以及 營造商 相關 紀錄   台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   周邊 拉起 警戒 線 提醒 民眾 注意安全   有民眾 警方 協助 下   回住 處 拿 東西   記者 林伯東 ／ 攝影 台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   周邊民眾 聚集 關心   記者 林伯東 ／ 攝影 台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   晚間 坑洞 正在 持續 灌漿   阻止 繼續 塌陷   記者 林伯東 ／ 攝影 台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   台北市 議員 許淑華   前右   到場 關心民眾   記者 林伯東 ／ 攝影 台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   台北 市長 蔣萬安   左二     台北市 議員 徐巧 芯   右二   到場 關心   記者 林伯東 ／ 攝影</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve">台北市 信義區 崇德 街巷 弄 13 日 下午 發生 路面 塌陷 事故   現場 緊鄰 一旁 建案 工地   中央社   台北市 信義區 一處 建案 旁 巷弄 今天下午 出現 長 15 公尺   深 3 公尺 坑洞   市府 表示   正在 持續 向 坑洞 灌漿   建案 基地 灌水   共 撤離 周遭 16 戶住 戶   其餘住 戶判斷 沒有 危險                           台北市 信義區 崇德 街巷 弄 今天下午 出現 一個 長 15 公尺   寬 3 公尺   深度 3 公尺 坑洞   道路 緊鄰 建築 基地 當時 正在 施作 連續 壁 工程   目前 已 停工 並 疏散 鄰近 住戶   副 市長 李 四川   工務局 長 黃 一平   都 發局 長 王玉芬 皆 到場 了解 狀況     王玉芬 向 中央社 記者 表示   坑洞 正在 持續 灌漿   建築 基地 則用 消防 車 灌水   讓 內外 壓力 平衡   阻止 繼續 塌陷   何時 才能 確認 沒 進 一步 危害 則要 持續 觀察     至於 住戶 部分   王玉芬 說   已經 撤離 16 戶   其中 10 人 需要 安置   這些 開銷 都 會 由 開發 單位 負責   其餘住 戶 雖 由 台北市 結構 技師 公會 判斷 沒有 危險   考量 住戶 仍會 擔心   已 請里長 逐戶 安撫     談到 事發 過程   附近 居民 仍然 餘悸 猶存   鄭 大哥 說   他 姊姊 大概 下午 2 時 50 分 時候 聽 到   砰   聲音   並 看到 門口 出現 一個 小洞   就 喊 他 出去 看   洞 這個 過程 中越 來 越 大   路上 腳踏車   摩托 車等 就 跟 著 掉下去     很 可怕       鄭 大哥 表示   他 住 這裡 3 年 多 了   旁邊 建案 大概 去年 開始 施工   剛開 挖 時候 路面 龜裂   建商 就 來 補好   之 後 雖然 施工 時 住家 總會 感到 地震   無法 睡 午覺   但 沒 什麼 異狀     黃 則說   他 住 這裡 20 多年 了   今天下午 外面 散步   走過 去 時 發現 一個 小洞   這個 洞後來 持續 陷 下去   但 他 沒 聽 到 什麼 聲音     新竹縣 竹北 莊敬 六街 一處 建案 周邊 日前 才 發生 路基 坍塌   導致 一輛 停放 路邊 特斯拉 轎車 直接 掉落  </t>
+          <t xml:space="preserve">台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   台北 市長 蔣萬安   中   到場 關心   記者 林伯東 ／ 攝影 台北市 信義區 崇德 街今   13   日 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   且 二度 坍塌   台北 市長 蔣萬安 晚上 到場 關心並 作出 四點 指示       蔣萬安 表示   市府 已 第一 時間 做出 相關 緊急 疏散 處置   並向 同仁 作出 四點 指示                             第一   安全 至上       相關 緊急 應變 處置 必 須 儘 速 地 完成   包括 疏散   安置 等   已 媒合 旅宿業 進行 安置   住民 入住 可依規定 申請 補助   我們 會 盡力將 損害 降到 最低       第二   釐 清 坍塌 原因   儘 快 排除       目前 了解 可能 是 連續 壁 滲水 問題   市府 會 儘 速 地 找出 造成 地面 坍塌 真正 原因   並 儘 快 排除   避免 坍塌 面積 持續 擴大       第三   事件 整體 調查       就 這次 地面 坍塌 事件   將針 對 工地 負責營 造商   就 過去 相關 建造 紀錄 整體 調查       第四   全市 工地 全面 清查       崇德 街案 緊急 處置 後   將針 對 台北市 興建 工程 工地 作 全面 清查   避免 相關 事件 重演       蔣萬安強 調   目前 已責成 相關 局處   務必 盡速 完成 相關 緊急應 變作 為   確 保住 民   市民 安全   避免 讓 地面 坍塌 損壞 再 持續 擴大   將損害 降到 最低   全力 捍衛 市民 生命 財產 安全       根據 建管處 資料 顯示   該起 工程 工地 起造 人 是 東禧 建設   承造 人 是 華熊 營造   監造 人 是 向度 聯 合建 築師 事務 所   目前 則已針 對 承造 人   監造 人 各 開罰 新 台幣 九萬元  </t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   台北 市長 蔣萬安   中   到場 關心   記者 林伯東 ／ 攝影     台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   台北 市長 蔣萬安 晚間 前往 現場                             蔣萬安 指出   整個 狀況 控制 住 以 後   會針 對 台北市 工地   全面 清查   是不是 這次 事件 類 似的 情況   再積 極處理       蔣萬安說   第一 時間 消防局 長 就 趕到 現場   共 啟用 13 輛 消防 車   2 輛救護車   36 位 消防 同仁 趕到 現場   第一 先緊 急 應變 處置   包括 疏散   安置 或者 是 其他 必要 作為   相關 局處 都 發局   建管處   警察局   區 公所   水處   瓦斯 公司 等等   都 現場   必須 要 盡速 完成 相關 緊急應 變作 為   來確 保人 員 安全   避免 讓 地面 坍塌 損壞 再 持續 擴大   把 整個 損害 降到 最低       蔣萬安 指出   工地 部分   市府 馬 上 勒令停工   找出 這次 地面 坍塌 原因   盡快 排除   避免 坍塌 面積 持續 擴大   這次 地層下陷 事件   整起 事件 會 完整 調查   並且 就 工地 全面 檢視   以及 營造商 相關 紀錄         【 中央社 ／ 台北 13 日電 】   北市 信義區 一處 建案 旁 巷弄 今天下午 出現 長 15 公尺   深 3 公尺 坑洞   市府 已 開罰 營造廠   建築師 各 9 萬元   市長 蔣萬安則 下令 後 續 要 清查 所有 工地   避免 類似 情況 再度 發生     台北市 信義區 崇德 街巷 弄 今天下午 約 3 時 突然 出現 一個 長 15 公尺   寬 3 公尺   深度 3 公尺 坑洞   下午 5 時 22 分 又 再度 塌陷   道路 緊鄰 新建 工地 當時 正在 施作 連續 壁 工程   市府 已 要求 停工 並 疏散 鄰近 16 戶住 戶     台北市 工務局 長 黃 一平   都 發局 長 王玉芬 皆 下午 4 時許 到場 了解 狀況   副 市長 李 四川 則在 晚間 6 時 抵達 現場   市長 蔣萬安約 晚間 6 時 30 分現 身     蔣萬安 聽取 報告 後 接受 媒體 聯訪 表示   消防局 下午 3 時許 獲報 地層下陷 後   共 出動 13 輛 消防 車   2 輛救護車 36 名 消防 員   消防局 長 莫懷祖 到場 坐鎮     蔣萬安說   第一件 事是 趕快 緊急 應變 處置   確 保人 員 都 安全   並 排除 事發 原因   避免 坍塌 再度 擴大   建築 工地 已 被 勒令停工     他 指出   接下 來會 就 這次 事件 完整 調查   全面 檢視 建築 工地 及營造 商紀錄   等 狀況 控制 住 後   會 清查 台北市 所有 工地   尤其 是 新建 工程 工地   避免 類似 情況 再度 發生     至於 需要 多久 處理 時間   蔣萬安說   目前 正積極 努力 中   同時 評估 要 不要 預防性 疏散   因為 市民 安全 最 重要   現場 關心 約 半小時 後   蔣萬安 晚間 6 時 50 分離開     台北市 結構 技師 公會 理事 長 徐茂卿 指出   因為 巷弄 旁邊 建案 地下 層連續 壁 破洞   導致 道路 塌陷   所以 緊急 撤離 周遭 住戶 後   在建 築 工地 灌水   道路 灌漿   讓 兩邊 土壓 平衡     現在 搶 救   原因 之後再 來 探討       台北市 建管處 表示   此 新建 工地 疑似 因施 作連續 壁時 滲水導致 道路 塌陷   將依建築法 第 89 條開罰 承造 人   營造廠     監造 人   建築師   各新 台幣 9 萬元   信義區 公所 表示   安置 需求者 每人每天 可申 請 新 台幣 1600 元 補助   最多 7 天       台北市 信義區 崇德 街巷 弄 道路 13 日驚傳 塌陷   警消 獲報 到場 疏散 鄰近 住戶   目前 無人 傷亡   但 現場 坍塌 似有 擴大 趨勢   傍晚 5 時許 現場 再度 塌陷   一旁 工地 藍色 帳棚 等 遭 波及 傾倒   中央社 台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   圖 ／ 消防局 提供</t>
+          <t>台北市 信義區 崇德 街 下午 出現 地層下陷   北市 府 表示   消防局 於 15 時 13 分通報   信義區 崇德 街 60 巷 22 號前 新建 工地 旁 道路 地層下陷   長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   無人 受傷       市府 表示   目前 處置 作為 已 疏散 鄰近 住戶   並劃 設 警戒 線   消防局 已先 成立 現場 指揮 站   建管處   新工處   道管 中心   瓦斯 公司   北水處 已 派員 趕 赴 現場 處理   信義區 區長 已 趕 抵 現場 坐鎮 指揮   目前 評估 約 10 餘位 住戶 需要 安置                             北市 信義區 出 現長 15 公尺   深 3 公尺   天坑     圖 ／ 北市 府 提供 北市 信義區 出 現長 15 公尺   深 3 公尺   天坑     圖 ／ 北市 府 提供</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>-1</v>
+        <v>30</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>北市 信義區 崇德 街 60 巷鄰近 一處 新建 工地   今天下午 3 點多 路面 突然 下陷   出現 一個 大 天坑   台北市 副 市長 李 四川   都 發局 長 王玉芬 傍晚 抵達 了解 現況   王 說 明處理 進度   住戶 方面 已 撤離 16 戶   工程 則在 坑洞 灌漿   建案 基地 灌水       都 發局 長 王玉芬 到場 表示   馬 路上 坑洞 約 10 幾 公尺 長   3 公尺 寬   深度 判斷 達 到 3 公尺   以 灌漿 方式 處理   建築 基地 開挖 地下室 部分   是 用 消防 水車 拉水線 灌水   使內外 壓力 可以 平衡   已拉 兩條 水線   再 請 消防局 再拉一條   加快 灌水 速度                             王玉芬 說 明住 戶 部分   已經 撤離 16 戶   10 人 需要 安置 且 安置 妥當 某 一家 旅館   所有 住宿   日常 開銷 都 會 由 營造 單位 負責   其餘住 戶 由 台北市 結構 技師 公會 判斷 沒有 危險   因 居民 擔心   請里長 逐戶 安撫   現場 分為 撤離區 監測區   除了 天坑 之外   轉角 一戶 地下室   技師 下去 看   目前 還沒有 任何 影響   會持續 監測       黃 住 當地 20 多年   他 提到 走路 經過 時   看到 裂一個 小洞   下午 2 點多 就 一直 下陷   從 22 號先 坍 下去   住戶 鄭 表示   他 姊姊 騎車 來 時   突然 聽到   砰   一聲 被 嚇到   那時 就 一個 小洞   自己 走 出去 看   前 後 不到 一分 鐘出 現好 大一個 洞 就 停住 了   沒 多久 警察 到場 就 要求 不要 過去   台北市 信義區 一處 新建 大樓 工地 旁 巷道 突然 塌陷   施工 單位 緊急 灌漿 回填   防止 塌陷 區域 擴大     記者 林俊良 ／ 攝影</t>
+          <t>北市 信義區 崇德 街 60 巷 路面 今天下午 出現 大 天坑   坑洞 長 15 公尺   寬 3 公尺   深度 2 到 3 公尺   機車   單車 陷落 坑中   消防局 已 疏散 鄰近 住戶 10 多人   台北市 建管處 表示   路面 坍陷 處以 混凝土 處置   目前 已 勒令停工   將依建築法 開罰 營造廠   監造 人 各 9 萬元       台北市 建管處 表示   事發地 旁為 一處 新建 住宅 大樓 工地   疑似 施作 連續 壁 滲水   導致 道路 塌陷   目前 以 混凝土 處置   工地 現場 緊急 處理 中   將依建築法 第 89 條開罰 承造 人   營造廠     監造 人   建築師   各 9 萬元   目前 已 勒令停工   未來 把 一切 安全 問題 妥善 完成 後 才 會 復工   消防局 已協助 將住 戶 全部 撤離 完畢   人員均 安全   信義區 公所 正在 處理 安置 問題                             北市 議員 許淑華 表示   該處 昨晚 就 灌水   疑似 連續 壁施作 釀禍   事發地 鄰近 住戶 共 30 戶   12 戶住 坍塌 處 附近   約 10 人 安置 飯店   要求 市府 妥善 協助 住戶   台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 ／ 翻攝 北市 信義區 出 現長 15 公尺 深 3 公尺   天坑     圖 ／ 北市 府 提供</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>北市 信義區 今 下午 3 點 多出 現大 天坑   崇德 街 60 巷 民宅 前 路面 坍陷   傍晚 5 點多 坑洞 再 擴大   消防局 已緊 急 疏散 鄰近 住戶   信義區 公所 區長 陳 冠伶 表示   9 位有 安置 需求者   已協助 找 好 旅社 並 入住   每人 每日 可申 請 補助 1600 元   最多 7 天       區長 陳 冠伶 表示   人數 調查 一直 變動   目前 9 位有 安置 需求   依規定 發生 緊急 災害 可 申請 安置 補助   每人 一天 1600 元   最多 申請 7 天   已協助 找 好 旅社   住戶 均 已 入住 安置   該 坑 主要 範圍 為 18 號至 24 號   警戒 區 12 號至 24 號已 拉起 封鎖線   台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 ／ 翻攝</t>
+          <t>台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   台北 市長 蔣萬安   中   到場 關心   記者 林伯東 ／ 攝影     台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   台北 市長 蔣萬安 晚間 前往 現場                             蔣萬安 指出   整個 狀況 控制 住 以 後   會針 對 台北市 工地   全面 清查   是不是 這次 事件 類 似的 情況   再積 極處理       蔣萬安說   第一 時間 消防局 長 就 趕到 現場   共 啟用 13 輛 消防 車   2 輛救護車   36 位 消防 同仁 趕到 現場   第一 先緊 急 應變 處置   包括 疏散   安置 或者 是 其他 必要 作為   相關 局處 都 發局   建管處   警察局   區 公所   水處   瓦斯 公司 等等   都 現場   必須 要 盡速 完成 相關 緊急應 變作 為   來確 保人 員 安全   避免 讓 地面 坍塌 損壞 再 持續 擴大   把 整個 損害 降到 最低       蔣萬安 指出   工地 部分   市府 馬 上 勒令停工   找出 這次 地面 坍塌 原因   盡快 排除   避免 坍塌 面積 持續 擴大   這次 地層下陷 事件   整起 事件 會 完整 調查   並且 就 工地 全面 檢視   以及 營造商 相關 紀錄         【 中央社 ／ 台北 13 日電 】   北市 信義區 一處 建案 旁 巷弄 今天下午 出現 長 15 公尺   深 3 公尺 坑洞   市府 已 開罰 營造廠   建築師 各 9 萬元   市長 蔣萬安則 下令 後 續 要 清查 所有 工地   避免 類似 情況 再度 發生     台北市 信義區 崇德 街巷 弄 今天下午 約 3 時 突然 出現 一個 長 15 公尺   寬 3 公尺   深度 3 公尺 坑洞   下午 5 時 22 分 又 再度 塌陷   道路 緊鄰 新建 工地 當時 正在 施作 連續 壁 工程   市府 已 要求 停工 並 疏散 鄰近 16 戶住 戶     台北市 工務局 長 黃 一平   都 發局 長 王玉芬 皆 下午 4 時許 到場 了解 狀況   副 市長 李 四川 則在 晚間 6 時 抵達 現場   市長 蔣萬安約 晚間 6 時 30 分現 身     蔣萬安 聽取 報告 後 接受 媒體 聯訪 表示   消防局 下午 3 時許 獲報 地層下陷 後   共 出動 13 輛 消防 車   2 輛救護車 36 名 消防 員   消防局 長 莫懷祖 到場 坐鎮     蔣萬安說   第一件 事是 趕快 緊急 應變 處置   確 保人 員 都 安全   並 排除 事發 原因   避免 坍塌 再度 擴大   建築 工地 已 被 勒令停工     他 指出   接下 來會 就 這次 事件 完整 調查   全面 檢視 建築 工地 及營造 商紀錄   等 狀況 控制 住 後   會 清查 台北市 所有 工地   尤其 是 新建 工程 工地   避免 類似 情況 再度 發生     至於 需要 多久 處理 時間   蔣萬安說   目前 正積極 努力 中   同時 評估 要 不要 預防性 疏散   因為 市民 安全 最 重要   現場 關心 約 半小時 後   蔣萬安 晚間 6 時 50 分離開     台北市 結構 技師 公會 理事 長 徐茂卿 指出   因為 巷弄 旁邊 建案 地下 層連續 壁 破洞   導致 道路 塌陷   所以 緊急 撤離 周遭 住戶 後   在建 築 工地 灌水   道路 灌漿   讓 兩邊 土壓 平衡     現在 搶 救   原因 之後再 來 探討       台北市 建管處 表示   此 新建 工地 疑似 因施 作連續 壁時 滲水導致 道路 塌陷   將依建築法 第 89 條開罰 承造 人   營造廠     監造 人   建築師   各新 台幣 9 萬元   信義區 公所 表示   安置 需求者 每人每天 可申 請 新 台幣 1600 元 補助   最多 7 天       台北市 信義區 崇德 街巷 弄 道路 13 日驚傳 塌陷   警消 獲報 到場 疏散 鄰近 住戶   目前 無人 傷亡   但 現場 坍塌 似有 擴大 趨勢   傍晚 5 時許 現場 再度 塌陷   一旁 工地 藍色 帳棚 等 遭 波及 傾倒   中央社 台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   圖 ／ 消防局 提供</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>台北市 出現 天坑   今天下午 15 時許   台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   坑洞 長 15 公尺   寬 3 公尺   深度 2 到 3 公尺   目視 可 看到 機車   自行 車 陷落 坑中   同時 坑洞 波及 一旁 民宅 地基   目前 台北市 消防局 已經 疏散 鄰近 住戶 10 多人   並劃 設緊 戒線   並 通知 市府 相關 單位 到場 處理       天坑 位 於 新建 工地 民宅 中間 巷弄 道路   塌陷 時 發出 聲響   驚動 住戶   但 因為 坑洞 擋 在家 門前   第一 時間 無法 脫困   消防局 緊急 到場   以 爬梯 方式 救援 住戶 出來                             消防局 救出 2 名 女子   疏散 1 男 1 女   人員 已 全數 疏散 完畢   另外 1 名 85 歲 老婦   因長 期行動 不便   雖無外傷   意識 清醒   但家屬 要求 預防性 送醫   由 消防局 送北醫   由 於 天坑 危及 安全   影響 周遭 至少 五戶 民宅   部分 住戶 無法 回家   估計 10 餘人受 影響   將由 台北市 府 處理 安置 問題       台北市 信義區 出現 天坑   目前 市府 新工處   建管處   勞檢處 等 相關 單位 都 已 派 人 到場   現場 設置 指揮 所   初步 懷疑 與 民宅 對面 新建 工地 工程 有關   現以 灌漿 方式 緊急 處置   至於 天坑 出現 原因   將 交由 市府 建管   新工 等 單位 調查   台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝</t>
+          <t>台北市 出現 天坑   今天下午 15 時許   台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   坑洞 長 15 公尺   寬 3 公尺   深度 2 到 3 公尺   目視 可 看到 機車   自行 車 陷落 坑中   同時 坑洞 波及 一旁 民宅 地基   目前 台北市 消防局 已經 疏散 鄰近 住戶   並劃 設緊 戒線   並 通知 府 相關 單位 到場 處理   台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   記者 廖炳棋 翻攝 台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   記者 廖炳棋 翻攝 台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   記者 廖炳棋 翻攝 台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   記者 廖炳棋 翻攝 台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   記者 廖炳棋 翻攝 台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   記者 廖炳棋 翻攝 台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   緊急 救援 住戶   圖 ／ 讀者 提供</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>-1</v>
+        <v>19</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>北市 信義區 崇德 街 60 巷 路面 今天下午 出現 大 天坑   坑洞 長 15 公尺   寬 3 公尺   深度 2 到 3 公尺   機車   單車 陷落 坑中   消防局 已 疏散 鄰近 住戶 10 多人   台北市 建管處 表示   路面 坍陷 處以 混凝土 處置   目前 已 勒令停工   將依建築法 開罰 營造廠   監造 人 各 9 萬元       台北市 建管處 表示   事發地 旁為 一處 新建 住宅 大樓 工地   疑似 施作 連續 壁 滲水   導致 道路 塌陷   目前 以 混凝土 處置   工地 現場 緊急 處理 中   將依建築法 第 89 條開罰 承造 人   營造廠     監造 人   建築師   各 9 萬元   目前 已 勒令停工   未來 把 一切 安全 問題 妥善 完成 後 才 會 復工   消防局 已協助 將住 戶 全部 撤離 完畢   人員均 安全   信義區 公所 正在 處理 安置 問題                             北市 議員 許淑華 表示   該處 昨晚 就 灌水   疑似 連續 壁施作 釀禍   事發地 鄰近 住戶 共 30 戶   12 戶住 坍塌 處 附近   約 10 人 安置 飯店   要求 市府 妥善 協助 住戶   台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 ／ 翻攝 北市 信義區 出 現長 15 公尺 深 3 公尺   天坑     圖 ／ 北市 府 提供</t>
+          <t>北市 信義區 崇德 街 60 巷鄰近 一處 新建 工地   今天下午 3 點多 路面 突然 下陷   出現 一個 大 天坑   台北市 副 市長 李 四川   都 發局 長 王玉芬 傍晚 抵達 了解 現況   王 說 明處理 進度   住戶 方面 已 撤離 16 戶   工程 則在 坑洞 灌漿   建案 基地 灌水       都 發局 長 王玉芬 到場 表示   馬 路上 坑洞 約 10 幾 公尺 長   3 公尺 寬   深度 判斷 達 到 3 公尺   以 灌漿 方式 處理   建築 基地 開挖 地下室 部分   是 用 消防 水車 拉水線 灌水   使內外 壓力 可以 平衡   已拉 兩條 水線   再 請 消防局 再拉一條   加快 灌水 速度                             王玉芬 說 明住 戶 部分   已經 撤離 16 戶   10 人 需要 安置 且 安置 妥當 某 一家 旅館   所有 住宿   日常 開銷 都 會 由 營造 單位 負責   其餘住 戶 由 台北市 結構 技師 公會 判斷 沒有 危險   因 居民 擔心   請里長 逐戶 安撫   現場 分為 撤離區 監測區   除了 天坑 之外   轉角 一戶 地下室   技師 下去 看   目前 還沒有 任何 影響   會持續 監測       黃 住 當地 20 多年   他 提到 走路 經過 時   看到 裂一個 小洞   下午 2 點多 就 一直 下陷   從 22 號先 坍 下去   住戶 鄭 表示   他 姊姊 騎車 來 時   突然 聽到   砰   一聲 被 嚇到   那時 就 一個 小洞   自己 走 出去 看   前 後 不到 一分 鐘出 現好 大一個 洞 就 停住 了   沒 多久 警察 到場 就 要求 不要 過去   台北市 信義區 一處 新建 大樓 工地 旁 巷道 突然 塌陷   施工 單位 緊急 灌漿 回填   防止 塌陷 區域 擴大     記者 林俊良 ／ 攝影</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>台北市 信義區 一處 新建 工地 旁 道路 地層下陷   崇德 街 60 巷 路面 今天下午 3 點 13 分出 現長 15 公尺   寬 3 公尺   約 2 至 3 公尺 深 大 天坑   台北市 建管處 表示   該案 因連續 壁施作   已 派員至 現場 了解 處理 中   目前 了解 是 連續 壁 滲水   工地 正在 止水 當中   消防局 現場 協助 鄰 房民眾 疏散   台北市 建管處 表示   該案 因連續 壁施作   已 派員至 現場 了解 處理 中   工地 正在 止水 當中   圖 ／ 讀者 提供 台北市 信義區 一處 新建 工地 旁 道路 地層下陷   崇德 街 60 巷 路面 出現 大 天坑   圖 ／ 讀者 提供</t>
+          <t xml:space="preserve">台北市 信義區 崇德 街巷 弄 13 日 下午 發生 路面 塌陷 事故   現場 緊鄰 一旁 建案 工地   中央社   台北市 信義區 一處 建案 旁 巷弄 今天下午 出現 長 15 公尺   深 3 公尺 坑洞   市府 表示   正在 持續 向 坑洞 灌漿   建案 基地 灌水   共 撤離 周遭 16 戶住 戶   其餘住 戶判斷 沒有 危險                           台北市 信義區 崇德 街巷 弄 今天下午 出現 一個 長 15 公尺   寬 3 公尺   深度 3 公尺 坑洞   道路 緊鄰 建築 基地 當時 正在 施作 連續 壁 工程   目前 已 停工 並 疏散 鄰近 住戶   副 市長 李 四川   工務局 長 黃 一平   都 發局 長 王玉芬 皆 到場 了解 狀況     王玉芬 向 中央社 記者 表示   坑洞 正在 持續 灌漿   建築 基地 則用 消防 車 灌水   讓 內外 壓力 平衡   阻止 繼續 塌陷   何時 才能 確認 沒 進 一步 危害 則要 持續 觀察     至於 住戶 部分   王玉芬 說   已經 撤離 16 戶   其中 10 人 需要 安置   這些 開銷 都 會 由 開發 單位 負責   其餘住 戶 雖 由 台北市 結構 技師 公會 判斷 沒有 危險   考量 住戶 仍會 擔心   已 請里長 逐戶 安撫     談到 事發 過程   附近 居民 仍然 餘悸 猶存   鄭 大哥 說   他 姊姊 大概 下午 2 時 50 分 時候 聽 到   砰   聲音   並 看到 門口 出現 一個 小洞   就 喊 他 出去 看   洞 這個 過程 中越 來 越 大   路上 腳踏車   摩托 車等 就 跟 著 掉下去     很 可怕       鄭 大哥 表示   他 住 這裡 3 年 多 了   旁邊 建案 大概 去年 開始 施工   剛開 挖 時候 路面 龜裂   建商 就 來 補好   之 後 雖然 施工 時 住家 總會 感到 地震   無法 睡 午覺   但 沒 什麼 異狀     黃 則說   他 住 這裡 20 多年 了   今天下午 外面 散步   走過 去 時 發現 一個 小洞   這個 洞後來 持續 陷 下去   但 他 沒 聽 到 什麼 聲音     新竹縣 竹北 莊敬 六街 一處 建案 周邊 日前 才 發生 路基 坍塌   導致 一輛 停放 路邊 特斯拉 轎車 直接 掉落  </t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>台北市 出現 天坑   今天下午 15 時許   台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   坑洞 長 15 公尺   寬 3 公尺   深度 2 到 3 公尺   目視 可 看到 機車   自行 車 陷落 坑中   同時 坑洞 波及 一旁 民宅 地基   目前 台北市 消防局 已經 疏散 鄰近 住戶   並劃 設緊 戒線   並 通知 府 相關 單位 到場 處理   台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   記者 廖炳棋 翻攝 台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   記者 廖炳棋 翻攝 台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   記者 廖炳棋 翻攝 台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   記者 廖炳棋 翻攝 台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   記者 廖炳棋 翻攝 台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   記者 廖炳棋 翻攝 台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   緊急 救援 住戶   圖 ／ 讀者 提供</t>
+          <t xml:space="preserve">【 17   27 ｜ 更新 天坑 初步 原因 】 信義區 崇德 街今   13   天 下午 3 點 13 分   傳出 一處 新建 案 工地 旁 道路   地層下陷     消防局 獲報 緊急 疏散 鄰近 住戶   無人 受傷   根據 消防局 獲報 消息   信義區 崇德 街 60 巷 22 號前 新建 工地 旁   出現 道路 地層下陷   馬 路上 出現 一個 長 15 公尺   寬 3 公尺   深度 約 4 公尺 天坑   摩托 車   腳踏車 都 掉入 坑洞   一旁 住戶 家門口 更是 危險   懸空     警消 人員 疏散 鄰近 住戶   所幸 無人 受傷   目前 劃設 警戒 線   建管處   新工處   道管 中心   瓦斯 公司   北水處 派員 趕 赴 現場 處理   信義區 區長 已 趕 抵 現場 坐鎮 指揮   目前 評估 約 10 餘位 住戶 需要 安置   這個 天坑 幾乎 占據 整條 巷弄   北市 建管處 初步 了解   由 於 住 戶 旁 就是 工地 施工   疑似 因為 工地 連續 壁施作   且 出現 滲水 狀況   才 釀成 天坑 出現   稍早 水泥 車緊 急先 進行 灌漿 作業   主要 基本 填補 坑洞   受影響 住戶 透露   剛剛 一度 5 名住 戶 受困 屋子 裡   所幸 消防 員協助 救援   而 三戶 門口 前端 地基 被 掏空   住戶 非常 擔心 房屋 可能 會 倒塌   地基 到底 穩不穩固   住 裡面 到底 安 不 安全   今天 晚上 到底 要 住 哪裡 等 問題   不過 關於後續 賠償 等 都 還要 進 一步 釐 清  </t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>台北市 信義區 崇德 街 下午 出現 地層下陷   北市 府 表示   消防局 於 15 時 13 分通報   信義區 崇德 街 60 巷 22 號前 新建 工地 旁 道路 地層下陷   長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   無人 受傷       市府 表示   目前 處置 作為 已 疏散 鄰近 住戶   並劃 設 警戒 線   消防局 已先 成立 現場 指揮 站   建管處   新工處   道管 中心   瓦斯 公司   北水處 已 派員 趕 赴 現場 處理   信義區 區長 已 趕 抵 現場 坐鎮 指揮   目前 評估 約 10 餘位 住戶 需要 安置                             北市 信義區 出 現長 15 公尺   深 3 公尺   天坑     圖 ／ 北市 府 提供 北市 信義區 出 現長 15 公尺   深 3 公尺   天坑     圖 ／ 北市 府 提供</t>
+          <t xml:space="preserve">台北市 信義區 崇德 街今   13   日 下午 3 點 13 分   傳出 一處 新建 案 工地 旁 道路   地層下陷     馬 路上 出現 一個 長 15 公尺   寬 3 公尺   深度 約 4 公尺 天坑   摩托 車   腳踏車 都 掉入 坑洞   一旁 住戶 家門口 更是 危險   懸空     而 台北 市長 蔣萬安 稍早 前往 現場 勘查   受訪 時 表示   第一 時間 就 即刻 派員前 來   相關 單位 了 緊急 疏散   強調   當這次 事件 緊急 處置 告一段落 之 後   會 台北市 相關 工地 全面 清查   了解 是否 有類 似 這次 地面 坍塌 原因   積極 相關 處置   目前 對廠 商及 建築師 各 開罰 9 萬元   工地 勒令停工   蔣萬安 表示   初步 了解   聽 了 相關 單位 說明   我們 下午 3 點 13 分   消防局 接收 到 地方 反應 這邊 地層下陷   第一 時間 就 即刻 派員前 來   趕快 連絡 了 警察局   新工處   建管處   區 公所   自來 水處   瓦斯 公司   台電 等 相關 單位   了 緊急 疏散   蔣萬安 指出   跟 指揮官   相關 單位 來 說明   第一   人員 安全 最 重要   所以 相關 緊急 應變 處置 必須 盡速 完成   包括 疏散   安置 等等   將這次 地面 坍塌 可能 造成 損害 降到 最低   第二   就 旁邊 工地   目前 了解 可能 是 連續 壁 滲水 問題   已經 趕快 了 處理   盡速 找出 坍塌 原因   然後盡 快 排除   避免 坍塌 面積 持續 擴大   第三   會 就 這次 地面 坍塌 事件 進行 調查   當然 包括 工地 實施者   營造 商過 去 相關 紀錄   第四   當這次 事件 緊急 處置 告一段落 之 後   要 台北市 相關 工地 全面 清查   了解 是否 有類 似 這次 地面 坍塌 原因   要積 極來 相關 處置   蔣萬安 表示     我們 現在 已經 非常 努力 緊急 應變   處置   第一 時間 盡快 疏散 了 住戶   我 想 市民 朋友 安全 是 最 重要   目前 還在 緊急 處置   我 想 必要 話 我們 還是 希望 預防性 疏散     而 台北市 土木 技師 公會 理事 長 莊均緯 指出   還要 再 把 崩塌 孔洞 填補 完成   現在 還在 灌水 當中   水頭 差會 慢慢 達到 平衡   而 因 地質 條件屬 於 沙 跟 水   因此 擔心 擋 土 設施 破洞   只要 衝破 連續 壁 洞   勢必 擋 土 牆後面 會 崩塌   目前 要 把 崩塌 部分 用 混 泥土 灌足外   開 挖面 水平衡   只要 水 與 地下水位 一 平衡   土沙 部分 就 會靜止   就 不會 往開 挖面 流動   防止 二次 下陷   目前 搶救 可控 範圍   莊均緯 表示   通常 會 發生 這狀況   是 地面 本來 就 下陷   只是 下陷 又 再 造成 第二 崩塌   灌漿 部分 還是 從 最 底下 往上 灌   表層 部分 基本上 還是 有些 鬆 動   需要 等 水位 平衡 後   才能 達到 搶災 最終 停止 狀態   估計 應該 都 要 到 凌晨  </t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t xml:space="preserve">台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   台北 市長 蔣萬安   中   到場 關心   記者 林伯東 ／ 攝影 台北市 信義區 崇德 街今   13   日 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   且 二度 坍塌   台北 市長 蔣萬安 晚上 到場 關心並 作出 四點 指示       蔣萬安 表示   市府 已 第一 時間 做出 相關 緊急 疏散 處置   並向 同仁 作出 四點 指示                             第一   安全 至上       相關 緊急 應變 處置 必 須 儘 速 地 完成   包括 疏散   安置 等   已 媒合 旅宿業 進行 安置   住民 入住 可依規定 申請 補助   我們 會 盡力將 損害 降到 最低       第二   釐 清 坍塌 原因   儘 快 排除       目前 了解 可能 是 連續 壁 滲水 問題   市府 會 儘 速 地 找出 造成 地面 坍塌 真正 原因   並 儘 快 排除   避免 坍塌 面積 持續 擴大       第三   事件 整體 調查       就 這次 地面 坍塌 事件   將針 對 工地 負責營 造商   就 過去 相關 建造 紀錄 整體 調查       第四   全市 工地 全面 清查       崇德 街案 緊急 處置 後   將針 對 台北市 興建 工程 工地 作 全面 清查   避免 相關 事件 重演       蔣萬安強 調   目前 已責成 相關 局處   務必 盡速 完成 相關 緊急應 變作 為   確 保住 民   市民 安全   避免 讓 地面 坍塌 損壞 再 持續 擴大   將損害 降到 最低   全力 捍衛 市民 生命 財產 安全       根據 建管處 資料 顯示   該起 工程 工地 起造 人 是 東禧 建設   承造 人 是 華熊 營造   監造 人 是 向度 聯 合建 築師 事務 所   目前 則已針 對 承造 人   監造 人 各 開罰 新 台幣 九萬元  </t>
+          <t xml:space="preserve">〔 記者 蔡亞樺 ／ 台北 報導 〕 台北市 信義區 出現 天坑   台北市 消防局 下午 3 時 13 分接 獲通報   信義區 崇德 街 60 巷 22 號前 新建 工地 旁 道路 地層下陷   長 15 公尺   寬 3 公尺   深度 2 至 3 公尺     附近 住家 門口 2 部機車 一部 腳踏車 瞬間 掉 進 天坑   幸無人 受傷     台北市 政府 表示   目前 已 疏散 鄰近 住戶   並劃 設 警戒 線   消防局 已先 成立 現場 指揮 站   建管處   新工處   道管 中心   瓦斯 公司   北水處 已 派員 趕 赴 現場 處理   信義區 長 已 趕 抵 現場 坐鎮 指揮   目前 評估 約 10 餘位 住戶 需要 安置     台北市 建築 管理 處 表示   該案 因連續 壁施作   已 派員至 現場 了解 處理 中   目前 了解 是 連續 壁 滲水   工地 正在 止水 當中   消防局 現場 協助 鄰 房民眾 疏散  </t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   台北 市長 蔣萬安 晚上 到場 關心並 指出   整個 狀況 控制 住 以 後   會針 對 台北市 工地   全面 清查   是不是 這次 事件 類 似的 情況   再積 極處理       蔣萬安 表示   工地 部分   市府 馬 上 勒令停工   找出 這次 地面 坍塌 原因   盡快 排除   避免 坍塌 面積 持續 擴大   這次 地層下陷 事件   整起 事件 會 完整 調查   並且 就 工地 全面 檢視   以及 營造商 相關 紀錄   台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   周邊 拉起 警戒 線 提醒 民眾 注意安全   有民眾 警方 協助 下   回住 處 拿 東西   記者 林伯東 ／ 攝影 台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   周邊民眾 聚集 關心   記者 林伯東 ／ 攝影 台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   晚間 坑洞 正在 持續 灌漿   阻止 繼續 塌陷   記者 林伯東 ／ 攝影 台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   台北市 議員 許淑華   前右   到場 關心民眾   記者 林伯東 ／ 攝影 台北市 信義區 崇德 街 下午 出現 地層下陷   天坑 長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   台北 市長 蔣萬安   左二     台北市 議員 徐巧 芯   右二   到場 關心   記者 林伯東 ／ 攝影</t>
+          <t>北市 信義區 今 下午 3 點 多出 現大 天坑   崇德 街 60 巷 民宅 前 路面 坍陷   傍晚 5 點多 坑洞 再 擴大   消防局 已緊 急 疏散 鄰近 住戶   信義區 公所 區長 陳 冠伶 表示   9 位有 安置 需求者   已協助 找 好 旅社 並 入住   每人 每日 可申 請 補助 1600 元   最多 7 天       區長 陳 冠伶 表示   人數 調查 一直 變動   目前 9 位有 安置 需求   依規定 發生 緊急 災害 可 申請 安置 補助   每人 一天 1600 元   最多 申請 7 天   已協助 找 好 旅社   住戶 均 已 入住 安置   該 坑 主要 範圍 為 18 號至 24 號   警戒 區 12 號至 24 號已 拉起 封鎖線   台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 ／ 翻攝</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>台北市 信義區 一處 新建 大樓 工地 旁 巷道   蹋陷   緊急 灌漿 回填   住戶 驚慌 撤離         消防局 於 15 時 13 分獲報   信義區 崇德 街 60 巷 22 號前 新建 工地 旁 道路 地層下陷 ( 長 15 公尺   寬 3 公尺   深度 2   3 公尺 )   幸無人 受傷                             警消 緊急 疏散 鄰近 住戶   並劃 設 警戒 線   消防局 已先 成立 現場 指揮 站   建管處   新工處   道管 中心   瓦斯 公司   北水處 已 派員 趕 赴 現場 處理   目前 評估 約 10 餘位 住戶 需要 安置   台北市 信義區 一處 新建 大樓 工地 旁 巷道 突然 塌陷   施工 單位 緊急 灌漿 回填   防止 塌陷 區域 擴大     記者 林俊良 ／ 攝影警 消緊 急 疏散 鄰近 住戶   並劃 設 警戒 線   消防局 已先 成立 現場 指揮 站   目前 評估 約 10 餘位 住戶 需要 安置   記者 林俊良 ／ 攝影 消防局 於 15 時 13 分獲報   信義區 崇德 街 60 巷 22 號前 新建 工地 旁 道路 地層下陷   警消 緊急 疏散 鄰近 住戶   並劃 設 警戒 線   消防局 已先 成立 現場 指揮 站   建管處   新工處   道管 中心   瓦斯 公司   北水處 已 派員 趕 赴 現場 處理   記者 林俊良 ／ 攝影 今天下午 台北市 信義區 一處 新建 大樓 工地 旁 巷道   突然 塌陷   住戶 心有 餘悸 驚慌 撤離   到 一旁 安全 區域   記者 林俊良 ／ 攝影 今天下午 台北市 信義區 一處 新建 大樓 工地 旁 巷道   突然 塌陷   警方 疏導 住戶 驚慌 撤離   目前 評估 約 10 餘位 住戶 需要 安置   記者 林俊良 ／ 攝影 台北市 信義區 一處 新建 大樓 工地 旁 巷道 突然 塌陷   施工 單位 緊急 灌漿 回填   防止 塌陷 區域 擴大     記者 林俊良 ／ 攝影</t>
+          <t>台北市 信義區 一處 新建 工地 旁 道路 地層下陷   崇德 街 60 巷 路面 今天下午 3 點 13 分出 現長 15 公尺   寬 3 公尺   約 2 至 3 公尺 深 大 天坑   台北市 建管處 表示   該案 因連續 壁施作   已 派員至 現場 了解 處理 中   目前 了解 是 連續 壁 滲水   工地 正在 止水 當中   消防局 現場 協助 鄰 房民眾 疏散   台北市 建管處 表示   該案 因連續 壁施作   已 派員至 現場 了解 處理 中   工地 正在 止水 當中   圖 ／ 讀者 提供 台北市 信義區 一處 新建 工地 旁 道路 地層下陷   崇德 街 60 巷 路面 出現 大 天坑   圖 ／ 讀者 提供</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -847,7 +847,7 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>-1</v>
+        <v>25</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -857,7 +857,7 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -867,7 +867,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -877,7 +877,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -897,7 +897,7 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -957,7 +957,7 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -967,7 +967,7 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -977,7 +977,7 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -987,7 +987,7 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -1007,27 +1007,27 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t xml:space="preserve">〔 記者 詹士弘 ／ 雲林 報導 〕 全國 最 嚴重 高鐵 地層下陷區 雲林 土庫 石廟 里   位 於 土庫 國中 附近 高鐵橋 下 道   路面 龜裂   坑坑洞洞   路況 極差   但 因 工程 涉及 鐵路 禁限 建範圍   須依   鐵路 兩側 禁建限建 辦法   規定 辦理   日前 終獲 高鐵局 同意   預計以 50 個 日 曆 天 完成 改善     土庫 鎮鎮長 陳 特凱 表示   石廟 里 高鐵橋 下 道路   經長 年 使用   平時車 流量 極大   加上 重車 違規 行駛   造成 路面 凹陷   破損 不堪   導致 居民 行車 時 容易 引發 交通事故   嚴 重影 響行車 安全   所以 向 縣府 反映   希望 能 儘 速 改善     高鐵土庫 段 是 高鐵 沿線 地層下陷 最 嚴重 地方   每年 平均 下陷 6.5 公分   工務 處長 汪令堯 表示   道 位 高鐵 正下方   涉及 鐵路 禁限建   範圍   須依   鐵路 兩側 禁建限建 辦法   規定 辦理   故 改為 專案 發包 方式 辦理   由 於 該 路段 交通量 極大   雖然限 10 噸 以下 車輛 行駛   但 還是 很多 重車 違規   加上 道路 路基 鬆 軟   所以 路況 極差     汪令堯 指出   由 於 道路 位 地層下陷區   加上 原先 就是 農地   土 質 鬆 軟   光重 鋪 路面   一下 大雨   重車 再 輾壓   道路 很快 就 會 再度 損壞   所以 需地質 改良   但 高鐵局 不 同意 用 給配 改善 路基   所以 工務處 改用 低 強度 水泥 替代   終獲 同意     汪令堯 表示   道路 改善 工程 總 預算 390 萬元   預期 改善 道路 長 度 兩側 約 630 公尺   寬 4.7 公尺   預計 9 月 中旬 發包   工期 為 50 日 曆 天   改善 後 可 提 昇 居民 生活 品質   維護用 路 人行 車安   另 他 會 建議 警察局   多派 員取 締重車 違規 行駛   才能 確保 道路 改善 後   以維持 好 行車 品質  </t>
+          <t>雲林縣 土庫 鎮高鐵 沿線 列屬 地層下陷 管制 區   高鐵 下方 雲 158 甲 通往 雲 97 線 道   雖 只 短短 約 500 公尺   但車 流大 路面 受損 累累   雲林縣 府 以 專案 經向 高鐵局 申請 修繕 獲准   將以 不 影響 高鐵 地基 安全 低 強度   高流動 建材 施工   預定 近期 封路 動工   10 月 完工       高鐵 雲林縣 土庫 段 受 地層下陷 影響   過去 以 每年 約 6.5 公分 沈陷 量 下陷   為維護 高鐵 安全   多年 前 曾 下陷區 動工將 橫跨 高鐵 台 78 線 快速道路   原為 土方 高架 改以 輕質 建材   重新 施工 進行   減重     此外   高鐵 沿線禁 抽 地下水   推廣 旱作 廣闢 黃 金 廊道   才 使 高鐵 雲林 段 沈陷 獲得 紓 緩                             位 於 土庫 高鐵 下方   連接 雲 158 甲及 雲 97 線 公路 高鐵 道   雖僅 短短 約 500 公尺   卻 是 管制 區內 唯一 高鐵 通道   土庫 鎮長 陳 特凱 說   高鐵 道 開通 多年   車流 大 卻 未曾 修繕   路面 凹陷 破損 累累   影響 行車 安全   居民 陳 情 希望 改善       雲林縣 長 張麗善 今天 會 同工 務處 縣 議員 王鈺齊   張維心 等 人現 勘   張麗善 說   道 位 於 高鐵 管制 區   不能 任意 挖掘 施工   因此 工務處 以 專案 計畫 向 高鐵局 申請 修繕   預定 今年 9 月 動工   10 月 完工   提供 平整 安全 道路   屆 時將 封路 約 50 天   請 車輛 繞 道       工務 處長 汪令堯 指出   高鐵下 道路 屬鐵路 禁限 建範圍   須依   鐵路 兩側 禁建限建 辦法   規定 辦理   未來 將以 390 萬元   對 高鐵下 寬 4.7 公尺 兩側 道 共 修繕 約 630 公尺   採   低 強度   高流動   混凝土 施工 法   打造 路基 更加 穩固       縣府 表示   為維護 高鐵 道 承載 安全   路口 設 有限 重 10 噸 以下 車輛 通行   但 地方 反映   長 期來 仍 不少 大型 車為求 方便 直接 通行   才 使 道路 面受損   將會 請 警方 加強 取締       隨後縣 長 張麗善 一行 人 再 轉往 土庫崙 雲 101   雲 98 道路 西螺 鎮九隆里 農路 等 會勘 改善 工程   雲林縣 長 張麗善 一行 人 再 轉往 土庫崙 等 地   會勘 多條 道路 工程   記者 蔡維斌 ／ 攝影 高鐵 雲林 土庫 段位 於 地層下陷 管制 區   高鐵下 唯一 道破 損 累累   經縣 府 向 高鐵局 專案 申請 後   近期 內將 封路 動工 修路   記者 蔡維斌 ／ 攝影</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>雲林縣 土庫 鎮高鐵 沿線 列屬 地層下陷 管制 區   高鐵 下方 雲 158 甲 通往 雲 97 線 道   雖 只 短短 約 500 公尺   但車 流大 路面 受損 累累   雲林縣 府 以 專案 經向 高鐵局 申請 修繕 獲准   將以 不 影響 高鐵 地基 安全 低 強度   高流動 建材 施工   預定 近期 封路 動工   10 月 完工       高鐵 雲林縣 土庫 段 受 地層下陷 影響   過去 以 每年 約 6.5 公分 沈陷 量 下陷   為維護 高鐵 安全   多年 前 曾 下陷區 動工將 橫跨 高鐵 台 78 線 快速道路   原為 土方 高架 改以 輕質 建材   重新 施工 進行   減重     此外   高鐵 沿線禁 抽 地下水   推廣 旱作 廣闢 黃 金 廊道   才 使 高鐵 雲林 段 沈陷 獲得 紓 緩                             位 於 土庫 高鐵 下方   連接 雲 158 甲及 雲 97 線 公路 高鐵 道   雖僅 短短 約 500 公尺   卻 是 管制 區內 唯一 高鐵 通道   土庫 鎮長 陳 特凱 說   高鐵 道 開通 多年   車流 大 卻 未曾 修繕   路面 凹陷 破損 累累   影響 行車 安全   居民 陳 情 希望 改善       雲林縣 長 張麗善 今天 會 同工 務處 縣 議員 王鈺齊   張維心 等 人現 勘   張麗善 說   道 位 於 高鐵 管制 區   不能 任意 挖掘 施工   因此 工務處 以 專案 計畫 向 高鐵局 申請 修繕   預定 今年 9 月 動工   10 月 完工   提供 平整 安全 道路   屆 時將 封路 約 50 天   請 車輛 繞 道       工務 處長 汪令堯 指出   高鐵下 道路 屬鐵路 禁限 建範圍   須依   鐵路 兩側 禁建限建 辦法   規定 辦理   未來 將以 390 萬元   對 高鐵下 寬 4.7 公尺 兩側 道 共 修繕 約 630 公尺   採   低 強度   高流動   混凝土 施工 法   打造 路基 更加 穩固       縣府 表示   為維護 高鐵 道 承載 安全   路口 設 有限 重 10 噸 以下 車輛 通行   但 地方 反映   長 期來 仍 不少 大型 車為求 方便 直接 通行   才 使 道路 面受損   將會 請 警方 加強 取締       隨後縣 長 張麗善 一行 人 再 轉往 土庫崙 雲 101   雲 98 道路 西螺 鎮九隆里 農路 等 會勘 改善 工程   雲林縣 長 張麗善 一行 人 再 轉往 土庫崙 等 地   會勘 多條 道路 工程   記者 蔡維斌 ／ 攝影 高鐵 雲林 土庫 段位 於 地層下陷 管制 區   高鐵下 唯一 道破 損 累累   經縣 府 向 高鐵局 專案 申請 後   近期 內將 封路 動工 修路   記者 蔡維斌 ／ 攝影</t>
+          <t xml:space="preserve">〔 記者 詹士弘 ／ 雲林 報導 〕 全國 最 嚴重 高鐵 地層下陷區 雲林 土庫 石廟 里   位 於 土庫 國中 附近 高鐵橋 下 道   路面 龜裂   坑坑洞洞   路況 極差   但 因 工程 涉及 鐵路 禁限 建範圍   須依   鐵路 兩側 禁建限建 辦法   規定 辦理   日前 終獲 高鐵局 同意   預計以 50 個 日 曆 天 完成 改善     土庫 鎮鎮長 陳 特凱 表示   石廟 里 高鐵橋 下 道路   經長 年 使用   平時車 流量 極大   加上 重車 違規 行駛   造成 路面 凹陷   破損 不堪   導致 居民 行車 時 容易 引發 交通事故   嚴 重影 響行車 安全   所以 向 縣府 反映   希望 能 儘 速 改善     高鐵土庫 段 是 高鐵 沿線 地層下陷 最 嚴重 地方   每年 平均 下陷 6.5 公分   工務 處長 汪令堯 表示   道 位 高鐵 正下方   涉及 鐵路 禁限建   範圍   須依   鐵路 兩側 禁建限建 辦法   規定 辦理   故 改為 專案 發包 方式 辦理   由 於 該 路段 交通量 極大   雖然限 10 噸 以下 車輛 行駛   但 還是 很多 重車 違規   加上 道路 路基 鬆 軟   所以 路況 極差     汪令堯 指出   由 於 道路 位 地層下陷區   加上 原先 就是 農地   土 質 鬆 軟   光重 鋪 路面   一下 大雨   重車 再 輾壓   道路 很快 就 會 再度 損壞   所以 需地質 改良   但 高鐵局 不 同意 用 給配 改善 路基   所以 工務處 改用 低 強度 水泥 替代   終獲 同意     汪令堯 表示   道路 改善 工程 總 預算 390 萬元   預期 改善 道路 長 度 兩側 約 630 公尺   寬 4.7 公尺   預計 9 月 中旬 發包   工期 為 50 日 曆 天   改善 後 可 提 昇 居民 生活 品質   維護用 路 人行 車安   另 他 會 建議 警察局   多派 員取 締重車 違規 行駛   才能 確保 道路 改善 後   以維持 好 行車 品質  </t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -1037,7 +1037,7 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -1127,27 +1127,27 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t xml:space="preserve">〔 記者 何玉華 ／ 台北 報導 〕 台北市 南港區 昨天 晚間 發生 道路 塌陷   經查 塌陷 原因 是 雨水 連 接管 脫管 造成   南港路 3 段 47 巷雙 向 封閉 施工   原 預計 今   19   晚 10 時 恢 復 通車   水利 處連夜 搶 修下   已 接續 完成 連 接管 脱管 處鋼 鈑 包覆   灌漿 回填 及路 面臨 鋪 作業   提前 於 早上 8 點開放 機車 小型 轎車 通行   預訂 中午 12 點 全面 通行     南港 警方 昨天 晚間 近 6 點 42 分   接獲 南港路 3 段 47 巷 與 昆陽街 60 巷 交叉路口 機車 停等區 地層下陷   下陷 面積長 約 2 公尺   寬約 2 公尺   深度 約 2 公尺   幸無人 受傷   員警劃 設 警戒 線   副 市長 李 四川 指示 區 公所   新工處 調派 重機 具開 挖   確認 坍塌 原因     經設 置 前進 指揮 所   水利 處 擴大開 挖 作業   確認 是 雨水 連 接管 脫管 造成   連夜 搶 修後已 經修 復 完成 並 回填 路面   今天 早上 已經 提前 恢 復 通車   後 續 新 工處 將會 以 透地雷達 檢測 無 其他 路面 下 空洞  </t>
+          <t>北市 南港路 3 段 47 巷   昆陽街 60 巷 交界   昨晚 出現 道路 局部 塌陷   連夜 搶 修下   預訂 中午 12 點 全面 通行       昨晚 天坑 地點 一處 機車 停等區   地層下陷 長 約 2 公尺   寬約 2 公尺   深度 約 2 公尺   由 水利 處派員 擔任 現場 指揮官   進行 擴大開 挖 作業                             水利 處 指出   連夜 搶 修下   已 接續 完成 連 接管 脱管 處鋼 鈑 包覆   灌漿 回填 及路 面臨 鋪 作業   19 日 8 時將 開放 機車 小型 轎車 通行   預訂 12 點 全面 通行   北市 天坑 搶修 完成   圖 北市 府 提供 北市 天坑 搶修 完成   圖 北市 府 提供</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>北市 南港路 3 段 47 巷   昆陽街 60 巷 交界   昨晚 出現 道路 局部 塌陷   連夜 搶 修下   預訂 中午 12 點 全面 通行       昨晚 天坑 地點 一處 機車 停等區   地層下陷 長 約 2 公尺   寬約 2 公尺   深度 約 2 公尺   由 水利 處派員 擔任 現場 指揮官   進行 擴大開 挖 作業                             水利 處 指出   連夜 搶 修下   已 接續 完成 連 接管 脱管 處鋼 鈑 包覆   灌漿 回填 及路 面臨 鋪 作業   19 日 8 時將 開放 機車 小型 轎車 通行   預訂 12 點 全面 通行   北市 天坑 搶修 完成   圖 北市 府 提供 北市 天坑 搶修 完成   圖 北市 府 提供</t>
+          <t xml:space="preserve">〔 記者 何玉華 ／ 台北 報導 〕 台北市 南港區 昨天 晚間 發生 道路 塌陷   經查 塌陷 原因 是 雨水 連 接管 脫管 造成   南港路 3 段 47 巷雙 向 封閉 施工   原 預計 今   19   晚 10 時 恢 復 通車   水利 處連夜 搶 修下   已 接續 完成 連 接管 脱管 處鋼 鈑 包覆   灌漿 回填 及路 面臨 鋪 作業   提前 於 早上 8 點開放 機車 小型 轎車 通行   預訂 中午 12 點 全面 通行     南港 警方 昨天 晚間 近 6 點 42 分   接獲 南港路 3 段 47 巷 與 昆陽街 60 巷 交叉路口 機車 停等區 地層下陷   下陷 面積長 約 2 公尺   寬約 2 公尺   深度 約 2 公尺   幸無人 受傷   員警劃 設 警戒 線   副 市長 李 四川 指示 區 公所   新工處 調派 重機 具開 挖   確認 坍塌 原因     經設 置 前進 指揮 所   水利 處 擴大開 挖 作業   確認 是 雨水 連 接管 脫管 造成   連夜 搶 修後已 經修 復 完成 並 回填 路面   今天 早上 已經 提前 恢 復 通車   後 續 新 工處 將會 以 透地雷達 檢測 無 其他 路面 下 空洞  </t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -1167,7 +1167,7 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -1177,7 +1177,7 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -1187,7 +1187,7 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -1197,7 +1197,7 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -1207,7 +1207,7 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>24</v>
+        <v>-1</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
@@ -1227,7 +1227,7 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -1237,27 +1237,27 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>14</v>
+        <v>-1</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>嘉義 縣 新港 鄉 5 日 下午 5 時 30 分發生 芮氏 規模 5.5 極淺層 地震   深度 8.5 公里   今   6   日 下午 高雄 又 發生 芮氏 規模 4.3 地震   地震 頻傳 讓 民眾 人心惶惶   而據 統計   我國 住宅 地震 基本 保險 截至 7 月底 止   投保 率約 37.53%   相當 於 約 580 萬住 戶 沒 地震 保險   住宅 地震 保險 基金 呼籲民眾 可 投保 住宅 地震 基本 保險   以 減輕 地震 災情 造成 之 財物 損失       台灣 位處環 太平洋 地震 帶   地震 發生 頻繁   為 使民眾 迅速 獲得 基本 地震 險 保障   住宅 地震 保險 基金 呼籲民眾 可 投保 住宅 地震 基本 保險   以 減輕 地震 災情 造成 之 財物 損失                             住宅 地震 保險 基金 表示   我國 住宅 地震 基本 保險 截至 2023 年 7 月底 止   以 全國戶數 922 萬戶計   投保 率約 37.53%   顯示 民眾 對 於 自身 住宅 財產 已 頗 具風險 意識   惟 仍 許多 屋主 尚未 投保   建議 應 即 早 投保   以 獲得 基本保障       住宅 地震 保險 基金 提醒   住宅 地震 基本 保險 保障 範圍 主要 包括 因 地震 震動   地震 引起 之火災   爆炸   山崩   地層下陷   滑動   開裂   決口   海嘯   海潮 高漲   洪水 等 危險 事故   造成 已 投保 住宅 地震 基本 保險 房屋 倒塌 或 不堪 居住 之   全損   損失 時   即可 取得 保險 金額理 賠及 臨時 住宿 費用       目前 保險 金額 最高 為 150 萬元   臨時 住宿 費用 為 20 萬元   保險 期間 為 一年期   每年 保費 1   350 元   相當 於 每日 只 需 3.7 元   即可 獲得 基本 地震 險 保障   🏠 udn 房地產   推薦 新聞     ▪   台南 1 預售 建案 疑營造 熱銷 假象 炒作   遭消 保官 嚴查     ▪   老 又 臭 沒人要   他 目睹 台北 老 公寓   看房 要 排隊     一堆 人 搶     ▪   天氣熱 但 電費 上 漲   高雄 人 推薦 1 降溫 神物   不用 開冷氣     ▪   換同坪數 新房   房屋 稅 3 千變 3 萬 4     他 哀號   貴到 快 哭 出來     ▪   借錢 買房   台積 輪班 工程 師   繳不出 頭期   全場 曝下場   穩死</t>
+          <t>高雄 仁武 區 今晚 9 時 30 分許   有民眾 發現 出現 一個 大 天坑   地點 就 永新 五街 永仁 街 路口 旁電線桿 周邊   高雄市 議員黃 飛鳳 獲報 隨即 到場 關心   並 通知 相關 單位 到場 協處   目前 高 市府 水利局 已調 派 機具 場開 挖 釐 清 下陷 肇因       由 於   天坑 發生 位置 就 電線桿 周圍   為 避免 電線桿 倒塌 造成 停電 意外   台灣 電力 公司 鳳山 營業 處 派員 前往 現場   暫以 吊桿 支撐 固定 電線桿   至於   地層下陷 肇因   水利局 人員 正在 現場 以管 挖 機具 進行 開 挖 調查                             仁武 分局 表示   因 路面 出現 坍塌 情事   為 安全 著想 避免 影響 用路 人   警方 獲報 後 已 將該 路段 封閉   經 水利局 挖開 查看   發現 不明 水源 流入 導致 地基 塌陷   屬 水利局 權責   遂 先行 填補 搶修   目前 水利局 污水 二科科長 張進 二 正在 現場 監督   台灣 電力 公司 鳳山 營業 處 暫以 吊桿 支撐 電線桿   避免 意外 發生 造成 停電   記者 古和純 ／ 翻攝 高雄 仁武 區出現 地層下陷   圖 ／ 取自 高雄市 議員黃 飛鳳個 人 臉書 高雄市 府 水利局 人員 現場 開 挖後填補 路面   記者 古和純 ／ 翻攝</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>高雄 仁武 區 今晚 9 時 30 分許   有民眾 發現 出現 一個 大 天坑   地點 就 永新 五街 永仁 街 路口 旁電線桿 周邊   高雄市 議員黃 飛鳳 獲報 隨即 到場 關心   並 通知 相關 單位 到場 協處   目前 高 市府 水利局 已調 派 機具 場開 挖 釐 清 下陷 肇因       由 於   天坑 發生 位置 就 電線桿 周圍   為 避免 電線桿 倒塌 造成 停電 意外   台灣 電力 公司 鳳山 營業 處 派員 前往 現場   暫以 吊桿 支撐 固定 電線桿   至於   地層下陷 肇因   水利局 人員 正在 現場 以管 挖 機具 進行 開 挖 調查                             仁武 分局 表示   因 路面 出現 坍塌 情事   為 安全 著想 避免 影響 用路 人   警方 獲報 後 已 將該 路段 封閉   經 水利局 挖開 查看   發現 不明 水源 流入 導致 地基 塌陷   屬 水利局 權責   遂 先行 填補 搶修   目前 水利局 污水 二科科長 張進 二 正在 現場 監督   台灣 電力 公司 鳳山 營業 處 暫以 吊桿 支撐 電線桿   避免 意外 發生 造成 停電   記者 古和純 ／ 翻攝 高雄 仁武 區出現 地層下陷   圖 ／ 取自 高雄市 議員黃 飛鳳個 人 臉書 高雄市 府 水利局 人員 現場 開 挖後填補 路面   記者 古和純 ／ 翻攝</t>
+          <t>嘉義 縣 新港 鄉 5 日 下午 5 時 30 分發生 芮氏 規模 5.5 極淺層 地震   深度 8.5 公里   今   6   日 下午 高雄 又 發生 芮氏 規模 4.3 地震   地震 頻傳 讓 民眾 人心惶惶   而據 統計   我國 住宅 地震 基本 保險 截至 7 月底 止   投保 率約 37.53%   相當 於 約 580 萬住 戶 沒 地震 保險   住宅 地震 保險 基金 呼籲民眾 可 投保 住宅 地震 基本 保險   以 減輕 地震 災情 造成 之 財物 損失       台灣 位處環 太平洋 地震 帶   地震 發生 頻繁   為 使民眾 迅速 獲得 基本 地震 險 保障   住宅 地震 保險 基金 呼籲民眾 可 投保 住宅 地震 基本 保險   以 減輕 地震 災情 造成 之 財物 損失                             住宅 地震 保險 基金 表示   我國 住宅 地震 基本 保險 截至 2023 年 7 月底 止   以 全國戶數 922 萬戶計   投保 率約 37.53%   顯示 民眾 對 於 自身 住宅 財產 已 頗 具風險 意識   惟 仍 許多 屋主 尚未 投保   建議 應 即 早 投保   以 獲得 基本保障       住宅 地震 保險 基金 提醒   住宅 地震 基本 保險 保障 範圍 主要 包括 因 地震 震動   地震 引起 之火災   爆炸   山崩   地層下陷   滑動   開裂   決口   海嘯   海潮 高漲   洪水 等 危險 事故   造成 已 投保 住宅 地震 基本 保險 房屋 倒塌 或 不堪 居住 之   全損   損失 時   即可 取得 保險 金額理 賠及 臨時 住宿 費用       目前 保險 金額 最高 為 150 萬元   臨時 住宿 費用 為 20 萬元   保險 期間 為 一年期   每年 保費 1   350 元   相當 於 每日 只 需 3.7 元   即可 獲得 基本 地震 險 保障   🏠 udn 房地產   推薦 新聞     ▪   台南 1 預售 建案 疑營造 熱銷 假象 炒作   遭消 保官 嚴查     ▪   老 又 臭 沒人要   他 目睹 台北 老 公寓   看房 要 排隊     一堆 人 搶     ▪   天氣熱 但 電費 上 漲   高雄 人 推薦 1 降溫 神物   不用 開冷氣     ▪   換同坪數 新房   房屋 稅 3 千變 3 萬 4     他 哀號   貴到 快 哭 出來     ▪   借錢 買房   台積 輪班 工程 師   繳不出 頭期   全場 曝下場   穩死</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
@@ -1267,7 +1267,7 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -1277,7 +1277,7 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
@@ -1297,7 +1297,7 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
@@ -1307,7 +1307,7 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
@@ -1317,7 +1317,7 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
@@ -1337,7 +1337,7 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
@@ -1357,27 +1357,27 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>-1</v>
+        <v>19</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>新竹市 和平 路竹 慶建設   筑光   建案 工地 下 挖 地下室   未料 前天 發生 基地 旁 道路 下方 自來 水管 線   瓦斯 管線 洩漏   連帶 造成 和平路 20 巷 地層下陷   由 於   天坑   填平 後   今天 又 他 處 塌陷   竹 市府 下午 成立 前進 指揮 所   市長 高虹安 提出 8 點 指示   包括 要求 廠商以 最快 速度 完成 對 周邊 民宅 自動 傾斜 偵測 設備 裝置 並即 時 回報   確保當 地 安全       和平路 該 建案 工地 規畫 地上 14 層   地下 3 層 建物   正在 下 挖 地下 3 層   前天 竟釀 緊鄰 巷弄 道路 下陷 後   被 市府 勒令停工   不過   因為 一旁 住家 距離 建案 基地 只有 3 公尺   將近 40 戶住 戶 對 道路 持續 下沉 塌陷 狀況 相當 擔憂   市府 今天下午 請來 4 大技師 公會 到場 會勘                             高虹安 今天 中午 下令 於 竹光國 中旁 成立 災害 應變 前進 指揮 所   並 要求 廠商 與 消防局   警察局   都 發處   民政 處   產發處   區 公所 立即 派員進 駐   下午 4 點半   高虹安 會 同 土木 技師 等 四大 專業 技師 公會 民富 里 沈朝 旺里長 聽取 簡報   並 了解 居民 訴求       高虹安 今晚 臉書 發文 說明   針對 此案 已下 達 8 項 指示   包含 責成 消防局   工務處 與 產發處 聯 繫 自 來 水 與 瓦斯 公司 明天 立即 進場 全面 開 挖汰 換成 最新 管線   因無法 同 時汰換 兩種 管線   將 依序 先後汰換 自來 水 與 瓦斯 管線       由 於 傾斜計 監測 數值 逼近 警戒 值   高虹安 要求 廠商以 最快 速度 完成 對 周邊 民宅 自動 傾斜 偵測 設備 裝置   並即 時 回報   要求 消防局 會同 民政 處   社會處 研擬 若事態 進 一步 擴大時   緊急 撤離 與 安置 措施   並預 準備       明天 開始 於 管線汰換 與 相關 改善 工程 期間   要求 廠商 每日 提供 足量 飲 用水 與 水車 供 停水 住戶 使用   要求 交通 處開放 周邊 停車場 供 居民 暫時 停放 車輛   竹光 國民運動 中心 免費 開放 居民 盥洗 使用       高虹安 說   確認 改善 完成 前   要求 災害 應變 前進 指揮 所 全天候 開設   隨時 提供 居民 諮 詢 與 處理 居民 回報 相關 問題   於 管線汰換 與 相關 改善 工程 期間   要求 警察局 做好 周邊 交通管制   確保 對 當地 交通 衝擊 降到 最低       高虹安說   今天 現場 與 當地 居民 溝通 與 聆 聽 心聲   並 一一 記錄   要求 廠商 與 局處 盡 全力 處理   強調 市府 團隊 一定 是 各位 最大 靠山   不僅會 要求 廠商 負起 責任   完成 改善 並經 確認 安全 無虞 之前   不得 進行 除了 安全工程 以外 其他 工程   新竹市 和平 路竹 慶建設   筑光   建案 工地 旁 和平路 20 巷 地層下陷   連日來 都 搶 修處理   記者 張裕珍 ／ 攝影 新竹 市長 高虹安 今天下午 到 和平路 20 巷 了解 居民 心聲   圖 ／ 竹 市府 提供 新竹 市長 高虹安 今天下午 進入 建案 基地 勘查 狀況   圖 ／ 竹 市府 提供 新竹市 和平 路竹 慶建設   筑光   建案 工地 旁 和平路 20 巷 地層下陷   連日來 都 搶 修處理   記者 張裕珍 ／ 攝影</t>
+          <t>新竹市 和平路 某建案 工地 下 挖 地下室   前天 發生 緊鄰 和平路 20 巷道 路 下陷   還有 自來 水洩漏   瓦斯 異味 飄散 情形   引起 住戶 疑慮   雖然 天坑 處緊 急 回填   但 仍 持續 他 處 下陷   建物 傾斜計 監測 數值 逼近 警戒 值   自來 水 公司 將於 明天 起汰換 上百 公尺 老舊 自來 水塑膠 管線   市長 高虹安 下午 赴 前進 指揮 所 了解 應變 情形       新竹市 和平路 該 建案 工地 規畫 地上 14 層   地下 3 層 建物   正在 下 挖 地下 3 層   未料 前天 竟釀 緊鄰 巷弄 道路 下陷   由 於 一旁 住家 距離 建案 基地 只有 3 公尺   將近 40 戶住 戶 相當 擔憂   市府 今天下午 請 來 4 大技師 公會 到場 了解   確認 工地 與 道路 下陷 情形                             據 了解   前天 發生 和平路 20 巷   天坑   事件 後   建商 取得 住戶 同意 20 巷前   中   後 段 設置 建物 傾斜計 監測 傾斜 情形   今天 最新 測得 最大值 每秒 387   已經 接近 每秒 413 警戒 值   由 於 和平路 20 巷 仍 道路 下陷   漏水 情形   今天 緊急 加裝 關水閥 處理       建案 營造 商工 務經理 黃 姓 經理 說   建案 地質 為 砂質 帶土   下 挖 施工 採鑽掘 方式 進行   強度 類似 連續 壁 工法   但蔽 體開 挖 壓力 造成 基地 外側 道路 內部 土壤 位移   加上 巷內 老舊 自來 水管 線 破裂   漏水 導致 土壤 泥沙 流失   進而 造成 地層下陷   水 流入 基地       由 於 和平路 20 巷內 約 3   40 戶 民宅   民富 里里長 沈朝旺 說   住戶 都 擔心 房子 會 塌陷   不要 等到 真正 傾斜 就 來 不及 了   希望 相關 單位 公告 監測 數據   並 加快 自來 水 與 瓦斯 管線汰換   自來 水 公司 明天 將進場 開 挖   汰換 鑄鐵管   盼 建商 同步 處理 好 地基         各項 資訊要 更 透明   讓 住 戶們 安心     楊姓 住戶 說   他 巷 住 了 20 年   其他 老住 戶 更 住 了 40 多年   大家 都 擔心 道路 下陷 擴大   希望 檢測 資訊 更加 透明   因為 他們 肉眼 看不到 傾斜 程度   很 需要 科技 儀器 來 幫忙 監測   數據 要 公開 讓 住 戶 都 了解       由 於 建案 工地 旁不斷 道路 下陷   建案 自行 組成 應變 中心   應變 中心 代表 允諾   已經 協調 明天 自來 水 公司 進場 換管   加派 人力 前   後 分頭 施工 情形 下   能 7 天汰管 完成   預計 10 月初 再換 瓦斯 管線   若 傾斜計 監測 到 了 警戒 值   將 安置 住戶 入住 旅館       新竹市 和平路 某建案 工地 下 挖 地下室   前天 發生 緊鄰 和平路 20 巷道 路 下陷   市府 今天 邀集 技師 公會 進入 工地 會勘   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室   造成 緊鄰 和平路 20 巷道 路 下陷   明天 將進 場汰換 老舊 自來 水管 線   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室 造成 緊鄰 和平路 20 巷道 路 下陷   市府 今天 設置 前進 指揮 所   市長 高虹安 下午 到場 了解 應變 情形   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室   前天 發生 緊鄰 和平路 20 巷道 路 下陷   市府 今天 邀集 技師 公會 進入 工地 會勘   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室 造成 緊鄰 和平路 20 巷道 路 下陷   市府 今天 設置 前進 指揮 所   市長 高虹安 下午 到場 了解 應變 情形   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室   前天 發生 緊鄰 和平路 20 巷道 路 下陷   市府 今天 邀集 技師 公會 進入 工地 會勘   記者 張裕珍 ／ 攝影</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>-1</v>
+        <v>19</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>新竹市 和平路 某建案 工地 下 挖 地下室   前天 發生 緊鄰 和平路 20 巷道 路 下陷   還有 自來 水洩漏   瓦斯 異味 飄散 情形   引起 住戶 疑慮   雖然 天坑 處緊 急 回填   但 仍 持續 他 處 下陷   建物 傾斜計 監測 數值 逼近 警戒 值   自來 水 公司 將於 明天 起汰換 上百 公尺 老舊 自來 水塑膠 管線   市長 高虹安 下午 赴 前進 指揮 所 了解 應變 情形       新竹市 和平路 該 建案 工地 規畫 地上 14 層   地下 3 層 建物   正在 下 挖 地下 3 層   未料 前天 竟釀 緊鄰 巷弄 道路 下陷   由 於 一旁 住家 距離 建案 基地 只有 3 公尺   將近 40 戶住 戶 相當 擔憂   市府 今天下午 請 來 4 大技師 公會 到場 了解   確認 工地 與 道路 下陷 情形                             據 了解   前天 發生 和平路 20 巷   天坑   事件 後   建商 取得 住戶 同意 20 巷前   中   後 段 設置 建物 傾斜計 監測 傾斜 情形   今天 最新 測得 最大值 每秒 387   已經 接近 每秒 413 警戒 值   由 於 和平路 20 巷 仍 道路 下陷   漏水 情形   今天 緊急 加裝 關水閥 處理       建案 營造 商工 務經理 黃 姓 經理 說   建案 地質 為 砂質 帶土   下 挖 施工 採鑽掘 方式 進行   強度 類似 連續 壁 工法   但蔽 體開 挖 壓力 造成 基地 外側 道路 內部 土壤 位移   加上 巷內 老舊 自來 水管 線 破裂   漏水 導致 土壤 泥沙 流失   進而 造成 地層下陷   水 流入 基地       由 於 和平路 20 巷內 約 3   40 戶 民宅   民富 里里長 沈朝旺 說   住戶 都 擔心 房子 會 塌陷   不要 等到 真正 傾斜 就 來 不及 了   希望 相關 單位 公告 監測 數據   並 加快 自來 水 與 瓦斯 管線汰換   自來 水 公司 明天 將進場 開 挖   汰換 鑄鐵管   盼 建商 同步 處理 好 地基         各項 資訊要 更 透明   讓 住 戶們 安心     楊姓 住戶 說   他 巷 住 了 20 年   其他 老住 戶 更 住 了 40 多年   大家 都 擔心 道路 下陷 擴大   希望 檢測 資訊 更加 透明   因為 他們 肉眼 看不到 傾斜 程度   很 需要 科技 儀器 來 幫忙 監測   數據 要 公開 讓 住 戶 都 了解       由 於 建案 工地 旁不斷 道路 下陷   建案 自行 組成 應變 中心   應變 中心 代表 允諾   已經 協調 明天 自來 水 公司 進場 換管   加派 人力 前   後 分頭 施工 情形 下   能 7 天汰管 完成   預計 10 月初 再換 瓦斯 管線   若 傾斜計 監測 到 了 警戒 值   將 安置 住戶 入住 旅館       新竹市 和平路 某建案 工地 下 挖 地下室   前天 發生 緊鄰 和平路 20 巷道 路 下陷   市府 今天 邀集 技師 公會 進入 工地 會勘   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室   造成 緊鄰 和平路 20 巷道 路 下陷   明天 將進 場汰換 老舊 自來 水管 線   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室 造成 緊鄰 和平路 20 巷道 路 下陷   市府 今天 設置 前進 指揮 所   市長 高虹安 下午 到場 了解 應變 情形   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室   前天 發生 緊鄰 和平路 20 巷道 路 下陷   市府 今天 邀集 技師 公會 進入 工地 會勘   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室 造成 緊鄰 和平路 20 巷道 路 下陷   市府 今天 設置 前進 指揮 所   市長 高虹安 下午 到場 了解 應變 情形   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室   前天 發生 緊鄰 和平路 20 巷道 路 下陷   市府 今天 邀集 技師 公會 進入 工地 會勘   記者 張裕珍 ／ 攝影</t>
+          <t>新竹市 和平 路竹 慶建設   筑光   建案 工地 下 挖 地下室   未料 前天 發生 基地 旁 道路 下方 自來 水管 線   瓦斯 管線 洩漏   連帶 造成 和平路 20 巷 地層下陷   由 於   天坑   填平 後   今天 又 他 處 塌陷   竹 市府 下午 成立 前進 指揮 所   市長 高虹安 提出 8 點 指示   包括 要求 廠商以 最快 速度 完成 對 周邊 民宅 自動 傾斜 偵測 設備 裝置 並即 時 回報   確保當 地 安全       和平路 該 建案 工地 規畫 地上 14 層   地下 3 層 建物   正在 下 挖 地下 3 層   前天 竟釀 緊鄰 巷弄 道路 下陷 後   被 市府 勒令停工   不過   因為 一旁 住家 距離 建案 基地 只有 3 公尺   將近 40 戶住 戶 對 道路 持續 下沉 塌陷 狀況 相當 擔憂   市府 今天下午 請來 4 大技師 公會 到場 會勘                             高虹安 今天 中午 下令 於 竹光國 中旁 成立 災害 應變 前進 指揮 所   並 要求 廠商 與 消防局   警察局   都 發處   民政 處   產發處   區 公所 立即 派員進 駐   下午 4 點半   高虹安 會 同 土木 技師 等 四大 專業 技師 公會 民富 里 沈朝 旺里長 聽取 簡報   並 了解 居民 訴求       高虹安 今晚 臉書 發文 說明   針對 此案 已下 達 8 項 指示   包含 責成 消防局   工務處 與 產發處 聯 繫 自 來 水 與 瓦斯 公司 明天 立即 進場 全面 開 挖汰 換成 最新 管線   因無法 同 時汰換 兩種 管線   將 依序 先後汰換 自來 水 與 瓦斯 管線       由 於 傾斜計 監測 數值 逼近 警戒 值   高虹安 要求 廠商以 最快 速度 完成 對 周邊 民宅 自動 傾斜 偵測 設備 裝置   並即 時 回報   要求 消防局 會同 民政 處   社會處 研擬 若事態 進 一步 擴大時   緊急 撤離 與 安置 措施   並預 準備       明天 開始 於 管線汰換 與 相關 改善 工程 期間   要求 廠商 每日 提供 足量 飲 用水 與 水車 供 停水 住戶 使用   要求 交通 處開放 周邊 停車場 供 居民 暫時 停放 車輛   竹光 國民運動 中心 免費 開放 居民 盥洗 使用       高虹安 說   確認 改善 完成 前   要求 災害 應變 前進 指揮 所 全天候 開設   隨時 提供 居民 諮 詢 與 處理 居民 回報 相關 問題   於 管線汰換 與 相關 改善 工程 期間   要求 警察局 做好 周邊 交通管制   確保 對 當地 交通 衝擊 降到 最低       高虹安說   今天 現場 與 當地 居民 溝通 與 聆 聽 心聲   並 一一 記錄   要求 廠商 與 局處 盡 全力 處理   強調 市府 團隊 一定 是 各位 最大 靠山   不僅會 要求 廠商 負起 責任   完成 改善 並經 確認 安全 無虞 之前   不得 進行 除了 安全工程 以外 其他 工程   新竹市 和平 路竹 慶建設   筑光   建案 工地 旁 和平路 20 巷 地層下陷   連日來 都 搶 修處理   記者 張裕珍 ／ 攝影 新竹 市長 高虹安 今天下午 到 和平路 20 巷 了解 居民 心聲   圖 ／ 竹 市府 提供 新竹 市長 高虹安 今天下午 進入 建案 基地 勘查 狀況   圖 ／ 竹 市府 提供 新竹市 和平 路竹 慶建設   筑光   建案 工地 旁 和平路 20 巷 地層下陷   連日來 都 搶 修處理   記者 張裕珍 ／ 攝影</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
@@ -1407,7 +1407,7 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
@@ -1427,7 +1427,7 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>-1</v>
+        <v>19</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
@@ -1457,7 +1457,7 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
@@ -1477,7 +1477,7 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
@@ -1487,7 +1487,7 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
@@ -1517,7 +1517,7 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
@@ -1537,47 +1537,47 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t xml:space="preserve">屏東 是 光電場 熱區 之一   正 上演 光電板 與 農民 搶 地爭 奪戰   光電業者 挨家 挨戶 以 誘人 租金 勸 說 地主 租地 種電   租地 種蓮霧 果農 只能 忍痛 看著 心血 被毀   斬斷 兒子 想 當青農 接班 願望   青農 自嘲 說   政府 寧可 把 地租 給業者 種電   不給 老 農一畝 田維生   青年 若當   漂鳥   回農村   肯定 變走 投無路   落翅仔         五十六 歲 鄭明偉 林邊   佳冬 鄉 租下 三座 蓮霧園   他 說   兩座 花 了 十多年 整理   收成 正漸 入 佳境   地主 竟 收回 種電   他 只能 忍痛 放棄   由 於 種蓮霧 要 手把手 長 期培養 技術   正在 念農校 兒子 雖 有心 接手   但 他 勸 兒子 算了   最好 另謀 出路                             農民控 國產署   為 賺 更 多 租金     屏東 沿海 不少 國有 財產 署名 下 新生 地   被 農 民用 於 種田   六十三 歲 楊寶秀 枋寮 寮 段種 芭樂   無奈說   種芭樂近 四十年   也繳 用地 補償 金給 國產署   一直 相安 無事   近年 數度 送件 申請 合法 承租 都 被 拒絕   後 來 光電業者 芭樂園 貼 告示 已 承租 種電   要 農民 及早 搬離   國產 署則 回覆 因 地層下陷 不利 耕作   要 轉作光 電場       六十多 歲 呂姓 老農 靠 這片 三分 地 蓮霧 園維生   他 說   國產署 明知 老農靠 種蓮霧 養家   寧可租 給光 電業者 賺 更 多   如果 沒地 可種     我 不但 要 吃 土   連農保 都 沒 了         面對 農民 控訴   國產署 南區 分署 屏東 辦 公室 指出   光電業者 依法 種電   並願意 取得 承租人 或 使用 人 同意 書 後 清理 地上 物   占用 者 繳 使用 補償 金   但 他們 本 就 沒 合法 使用 權       林邊   佳冬 枋寮   蓮霧 之 鄉   美名   四十八 歲 陳 呈祥 八八 風災後回 鄉 接手 父親 蓮霧園   他 感嘆   近年 光電大舉 入侵   正 侵蝕 果農 維 繫 傳 統 產 業 所 努力       他 說   蓮霧 老農因 子女 無意 接手   只好 租地 給光 電商   果園 地主 刻意 抬高 租金 逼退 承租 農   一塊 塊 果園 被 光電場 取代   包圍   整體 產量 正持續 下降   衝擊 採收   包裝   運銷 等 產業 鏈   未來 工人 更難 找   材料 更貴   務農條件 就 更 差       農地 租金 上漲   加速 產業 衰退     陳 呈祥 說   蓮霧 產業 衰退 人口老化   缺工 等 有關   雖 不能 全歸責 光電   但 確實 造成 農地 租金 上漲 問題   間接 加速 產業 衰退   政府 對 這些 衝突視 若 無睹   苦果 只 由 農民吞       枋寮 農會 總幹事 鄭晏昕   林邊 農會 總幹事 黃 金順 都 慨嘆   原盼 農電能 共生   如今 衝突 嚴重   地 驕傲 半世 紀的 蓮霧 產業   正因 光電 面臨 式微 危機       黃 金順 說   光電場 租金 一分 地四萬元   承租 農民頂 多出 得起 一萬元   相差 四倍   到 處 都 聽 到 地 主要 改 種電   年 輕人 想 返 鄉務農   無 低 租金 農地 可種     蓮霧 故鄉   金字招牌 正在 褪色       台大 農經 碩士 張靜玉 是 枋寮 蓮霧 農   眼看 鄰近 農民 被 光電 搶 地   忿忿不平   直指 當年 農委會 主委 蘇嘉全 還推 漂鳥 計畫   要 青年 返鄉務農   現在 連地 都 租 不到     這 不是 迫遷 青農去 都市 討 生活   漂鳥 回農村   恐怕 走 投無路 變 落翅仔    </t>
+          <t xml:space="preserve">聯合 報陽光 行動 專題 報導光 電進 駐 屏東   種電 範圍 遍及 農地   山區 到 文資 價值 二戰 遺跡   造成 家園 地景 地貌 變遷   衝擊 老 農生計   變相迫 遷青農   更 被 地方 形容 為   惡鄰     產生 蛇 鼠 與 害蟲   提升 鄰田 管理 困難度   還潛藏 糧食 危機     縣府 環保局 長 顏幸苑 表示   光電不會 無限 擴張   目前 種電 專區 仍 約 3 千公頃 可 耕作 並專案 輔導業者 除草   一定 會 兼顧 農業 永續 發展       顏幸苑 表示   台電饋 線 上限 規定   目前 既有 電力 設施 併 網 上限 下   限度 推動 光電 專區   不會 無 限制 使用 農地 種電   而 東港鎮   林邊   佳冬   枋寮 鄉 等 4 鄉鎮 專案 截至 去年底   共 併 網約 3 百 兆瓦 光電   該區 農地 總面 積約 3800 公頃   至少 還有 約 3 千公頃 面積 可 農作   使用 農地 比例 不到 4 鄉鎮 農地 總面積 一成                             強調   從 未 要求 廠商 提供   不利 耕作 同意 書   或 其他 不 平等 條約 相關 文件   針對 部分 地區 爭議 案件   未 取得 居民 同意 之前   皆 已 要求 業者 停止 施工   另太陽能 案場 內並 無 食物 來源   應非屬 引來 老鼠 主因   目前 已 要求 專案 輔導業者 定期 進行 除草   維護 周遭 環境 整潔       指出   屏東 綠能 推動 政策 以   專案 專區 計畫       土地 複 合式 利用   等 2 大 策略 為 優先   限度 使用 相對 不 適合 耕種 土地 發展 綠能   提供 給 地主   農民階段 性 活化 土地 新選擇   對 於 無力 管理 田間 工作   又 土地 鹽化 等 不利因素 無法 耕作 年 邁老農   則 可以 穩定 收入 過 退休 生活   至於 非 專案 專區 鄉鎮   則優先 鼓勵 廠 商以   土地 複 合式 利用   方式   利用 既有 設施 結合 太陽光 電設施   有效 利用 公共 空間       屏縣 府 綠能 辦 公室 表示   尊重 私有 地主 處置 自家 土地 財產   及業者 依法 申請 案件 權利   相關 審查 過程將 審慎 關注 山坡地   耕作 農地   歷史 遺跡   生態 保育 或 重要 觀 光景 點聯絡 道路 沿線 等 議題   並 要求 廠商 提出 因應 作為   以 避免 衍生 爭議性 問題   兼顧 開發 合理性 及維護 本縣 農民 耕作 權益       生利 能源 表示   屏東 枋寮 案場 是 合法 開發   於 2020 年 9 月 於 案場 發現 碉堡 等 歷史 遺構 後   隨即 保留 並主動展 開一連串 文資 保護作 為   並無二戰 槍堡 被 挖除 等 情事  </t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t xml:space="preserve">從國道 三號 林邊 交流 道 下來   光電場 廣告 映入 眼簾   從大馬 路旁 到 鄉間 農田   光電板 無 所 不   這是 屏東 沿海 地區 這幾年 興起 違 景致   是 全台 種電 縮影   地 青農批 政府   業者 聯手 種電 種到 失心 瘋   從 農地   山區 到 文資 價值 二戰 遺跡 都 不放過   不僅家園 變貌   迫使 老農離 農   變相迫 遷青農       屏東 農地 種光 電原 是 全台 濫觴 典範   二 九年 八月 莫 拉克 風災 挾帶 破紀錄 雨量   造成 中南部 嚴 重水 災   重創 屏東 南部 沿海 鄉鎮   不少 魚塭   果園 被 沖 毀   時任 屏東縣 長 曹啟 鴻 提出   養水 種電   計畫   縣府 媒合 魚塭   農地 租給 光電業者   地主 負責 管理   地主 按 月 收 地租 管理 費   綠電賣給 台電   能 涵養 地下水   減緩 下陷   一舉 數得                           屏東 種電   侵蝕 農地   製 表 ／ 都 會 地方 中心   農業部 前身 農委會 二 一 三年 修法   允許 不適 耕作 農地 種電   大開 種電 之門   但 農地 非農用 罵 聲不斷   二 一 八年 十月 起   屏縣 府 公告 實施   嚴重 地層下陷地區 土地 活化 暨 太陽光 電發 電業 整體 規劃 發展 計畫     開放 下陷區 農地 可 變更 種電       二 二 年 七月   農委會 加嚴 農地 變更 種電 門檻   二到卅公頃 農地 變更 要 由 中央 審查   兩公頃 以下 原則 不 同意 變更 種電   但 早 二 一 八年 屏東縣 長 潘孟安任   報請 行政院 同意 把 東港   林邊   佳冬   枋寮 四鄉鎮   畫為 嚴重 地層下陷區 作光電 專區   成為 特例       四年 多來   屏東 種電 發展 快速   原本 立意 良善 光電   如今 變成 農民 陰霾   枋寮 女青農 張靜玉 說   為衝 高綠電 占 比   種電 已種 到 失心 瘋   不該 種電 地方 都 被 光電板 占領   很多 農民 被 業者 遊說簽   不利 耕作 聲明書     離農 坐收 光電場 租金   但 這些 農地 都種 著蓮霧   水稻   芭樂   何來 不利 耕作         沿海 四鄉 鎮美麗 鄉間 景致 丕 變   綠地 逐漸 蒸發     屏東縣 環境 保護 聯盟 理事 長 洪輝祥 說   綠地   果園 被 一塊 塊 光電板 取代   像 貼 狗皮 膏藥般 醜陋   不但 壓縮 農業 空間   光電板 遮陽 廿年   農地 將 失去 地 力   衝擊 農產業 服務鏈   受益 是 少數 地主   受影響 是 多數 農民   整體 農業將 衰退   屆 時 想 回頭 搶 救 就 難 了       屏東縣 府 綠能 辦 公室 表示   沿海 四鄉 鎮持續 下陷   列 第一   二級 地下水 管制 區   縣府 把 四 鄉鎮 部分 農地 轉作光 電場   搭配 上游 補注 地下水   減緩 地層下陷   創造 地主   業者   政府   全民 與 綠能   五贏     前年 已達成 綠電供 應 全縣 民生 用電 階段 性 目標  </t>
+          <t xml:space="preserve">〔 記者 陳 彥廷 ／ 屏東 報導 〕 屏東縣 政府 於 東港   林邊   佳冬 枋寮 4 個 沿海 鄉鎮   劃定   嚴重 地層下陷區 光電計畫   專區   為確 保農民 耕作 權   不過   近來坊 間質 疑聲 浪漸 漲   環保局 強調   該區 計畫 發電量 為 800MW   百萬瓦     不會 無 限制 擴張   因此 至少 會 仍 3000 公頃 以上 農地 可供 農作     地面 型 光電場 成為 選戰 攻防 議題   屏東 因 沿海 嚴重 地層下陷區 為 全國 首個 縣府 核淮得 設光 電案場 專案   成 在野 黨攻 詰 對象   近期 坊 間 又 再 傳出 農民因 種電 失去 農保   老農 退場 又 留不住 青農及 蛇 鼠 窩 藏 副作用 等 爭議     屏縣 府 環保局 指出   這 4 鄉鎮過 去 因超 抽 地下水   曾列 為 嚴重 地層下陷區   現 仍屬 第 1   2 級 地下水 管制 區   且 海水 上溯 下   許多 土地 都 已 出現 鹽化   不少 已 是 不利 耕地 多年   因此 縣府 尊重 地主 利用 土地 意願 權益 前提 既有 電力 設施 併 網 上限 條件 下   限度 推動 光電 專區   預計 發電量 為 800MW     環保局 指出   部分 農地 轉作 太陽 光電 後   減少 農民 抽取 林邊 溪 下游 地下水 需求   並 搭配 上游 設置 大 潮州 人工湖 補注 地下水   減緩 地層下陷   達到 國土 復 育及 產業 永續 發展 目的   而 近年 同樣 大小 光電板 發電 效率 已較 八八 風災 後   養水 種電   到 近 2 倍   單 一片 就 可 發電達 400w   以 目前 併 網約 300MW 太陽光 電裝置 容量   使用 農地 比例 約 250 公頃 左右   未來 達 到 目標 單位 發電量 更大下   所 需面積 比例 一定 更 小   至少 會 3000 公頃 以上 農地 可供 農作 使用   另外   對 於 無力 管理 田間 工作   又 土地 鹽化 等 不利因素 無法 耕作 年 邁老農   則 可以 穩定 收入 過 退休 生活     至於 農保 問題   環保局 重申   農地 若 有意 願 出租 供 人 種電   一定 要 進行 變更 地目   但 這是 完全 基 於 地主 利用 土地 意願 權益   縣府 環保局 從 未 要求 廠商 提供 所謂   不利 耕作 同意 書   或 其他 網路 媒體 謠傳 不 平等 條約 相關 文件   先前 更 製 作 地主 注意 事項 手冊 Q &amp; A 圖卡   公告 於 縣府 綠辦 官網   讓 地主 了解 相關 權利 與 義務   只要 民眾 對 合約 疑問   均 可 撥 打 專線 電話詢 問綠能 專案 推動辦 公室   針對 部分 地區 爭議 案件   未 取得 居民 同意 之前   縣府 已 要求 業者 停止 施工     蛇鼠 患 問題   縣府 環保局 長 顏幸 苑則 認為   作物 收成 期間 食物 充沛 易 引鼠   鳥禽 覓 食   但 太陽能 案場 並無食源   應非屬 引鼠 主因   縣府 要求 專案 輔導業者 維護 周遭 環境 整潔   至於 選址 不當   縣府 重申   屏東縣 綠能 推動 政策 以   專案 專區 計畫       土地 複 合式 利用   兩大 策略 為主   專案 為 限度 使用 相對 不 適合 耕種 土地 發展 綠能   專案 專區 外 鄉鎮 優先 鼓勵 結合 既有 設施 與 光電   複 合 利用   方式     屏東縣 環保局 表示   民眾 對 於 光電 發展 與 環境 保護 議題 逐漸 重視   縣府 尊重 私有 地主 處置 自家 土地 財產   以及 業者 依法 申請 案件 權利   惟審查 過程將 審慎 關注 山坡地   耕作 農地   歷史 遺跡   生態 保育 或 重要 觀 光景 點聯絡 道路 沿線 等 議題   並 要求 廠商 提出 因應 作為   以 避免 衍生 爭議性 問題   兼顧 開發 合理性 及維護 本縣 農民 耕作 權益  </t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t xml:space="preserve">聯合 報陽光 行動 專題 報導光 電進 駐 屏東   種電 範圍 遍及 農地   山區 到 文資 價值 二戰 遺跡   造成 家園 地景 地貌 變遷   衝擊 老 農生計   變相迫 遷青農   更 被 地方 形容 為   惡鄰     產生 蛇 鼠 與 害蟲   提升 鄰田 管理 困難度   還潛藏 糧食 危機     縣府 環保局 長 顏幸苑 表示   光電不會 無限 擴張   目前 種電 專區 仍 約 3 千公頃 可 耕作 並專案 輔導業者 除草   一定 會 兼顧 農業 永續 發展       顏幸苑 表示   台電饋 線 上限 規定   目前 既有 電力 設施 併 網 上限 下   限度 推動 光電 專區   不會 無 限制 使用 農地 種電   而 東港鎮   林邊   佳冬   枋寮 鄉 等 4 鄉鎮 專案 截至 去年底   共 併 網約 3 百 兆瓦 光電   該區 農地 總面 積約 3800 公頃   至少 還有 約 3 千公頃 面積 可 農作   使用 農地 比例 不到 4 鄉鎮 農地 總面積 一成                             強調   從 未 要求 廠商 提供   不利 耕作 同意 書   或 其他 不 平等 條約 相關 文件   針對 部分 地區 爭議 案件   未 取得 居民 同意 之前   皆 已 要求 業者 停止 施工   另太陽能 案場 內並 無 食物 來源   應非屬 引來 老鼠 主因   目前 已 要求 專案 輔導業者 定期 進行 除草   維護 周遭 環境 整潔       指出   屏東 綠能 推動 政策 以   專案 專區 計畫       土地 複 合式 利用   等 2 大 策略 為 優先   限度 使用 相對 不 適合 耕種 土地 發展 綠能   提供 給 地主   農民階段 性 活化 土地 新選擇   對 於 無力 管理 田間 工作   又 土地 鹽化 等 不利因素 無法 耕作 年 邁老農   則 可以 穩定 收入 過 退休 生活   至於 非 專案 專區 鄉鎮   則優先 鼓勵 廠 商以   土地 複 合式 利用   方式   利用 既有 設施 結合 太陽光 電設施   有效 利用 公共 空間       屏縣 府 綠能 辦 公室 表示   尊重 私有 地主 處置 自家 土地 財產   及業者 依法 申請 案件 權利   相關 審查 過程將 審慎 關注 山坡地   耕作 農地   歷史 遺跡   生態 保育 或 重要 觀 光景 點聯絡 道路 沿線 等 議題   並 要求 廠商 提出 因應 作為   以 避免 衍生 爭議性 問題   兼顧 開發 合理性 及維護 本縣 農民 耕作 權益       生利 能源 表示   屏東 枋寮 案場 是 合法 開發   於 2020 年 9 月 於 案場 發現 碉堡 等 歷史 遺構 後   隨即 保留 並主動展 開一連串 文資 保護作 為   並無二戰 槍堡 被 挖除 等 情事  </t>
+          <t xml:space="preserve">從國道 三號 林邊 交流 道 下來   光電場 廣告 映入 眼簾   從大馬 路旁 到 鄉間 農田   光電板 無 所 不   這是 屏東 沿海 地區 這幾年 興起 違 景致   是 全台 種電 縮影   地 青農批 政府   業者 聯手 種電 種到 失心 瘋   從 農地   山區 到 文資 價值 二戰 遺跡 都 不放過   不僅家園 變貌   迫使 老農離 農   變相迫 遷青農       屏東 農地 種光 電原 是 全台 濫觴 典範   二 九年 八月 莫 拉克 風災 挾帶 破紀錄 雨量   造成 中南部 嚴 重水 災   重創 屏東 南部 沿海 鄉鎮   不少 魚塭   果園 被 沖 毀   時任 屏東縣 長 曹啟 鴻 提出   養水 種電   計畫   縣府 媒合 魚塭   農地 租給 光電業者   地主 負責 管理   地主 按 月 收 地租 管理 費   綠電賣給 台電   能 涵養 地下水   減緩 下陷   一舉 數得                           屏東 種電   侵蝕 農地   製 表 ／ 都 會 地方 中心   農業部 前身 農委會 二 一 三年 修法   允許 不適 耕作 農地 種電   大開 種電 之門   但 農地 非農用 罵 聲不斷   二 一 八年 十月 起   屏縣 府 公告 實施   嚴重 地層下陷地區 土地 活化 暨 太陽光 電發 電業 整體 規劃 發展 計畫     開放 下陷區 農地 可 變更 種電       二 二 年 七月   農委會 加嚴 農地 變更 種電 門檻   二到卅公頃 農地 變更 要 由 中央 審查   兩公頃 以下 原則 不 同意 變更 種電   但 早 二 一 八年 屏東縣 長 潘孟安任   報請 行政院 同意 把 東港   林邊   佳冬   枋寮 四鄉鎮   畫為 嚴重 地層下陷區 作光電 專區   成為 特例       四年 多來   屏東 種電 發展 快速   原本 立意 良善 光電   如今 變成 農民 陰霾   枋寮 女青農 張靜玉 說   為衝 高綠電 占 比   種電 已種 到 失心 瘋   不該 種電 地方 都 被 光電板 占領   很多 農民 被 業者 遊說簽   不利 耕作 聲明書     離農 坐收 光電場 租金   但 這些 農地 都種 著蓮霧   水稻   芭樂   何來 不利 耕作         沿海 四鄉 鎮美麗 鄉間 景致 丕 變   綠地 逐漸 蒸發     屏東縣 環境 保護 聯盟 理事 長 洪輝祥 說   綠地   果園 被 一塊 塊 光電板 取代   像 貼 狗皮 膏藥般 醜陋   不但 壓縮 農業 空間   光電板 遮陽 廿年   農地 將 失去 地 力   衝擊 農產業 服務鏈   受益 是 少數 地主   受影響 是 多數 農民   整體 農業將 衰退   屆 時 想 回頭 搶 救 就 難 了       屏東縣 府 綠能 辦 公室 表示   沿海 四鄉 鎮持續 下陷   列 第一   二級 地下水 管制 區   縣府 把 四 鄉鎮 部分 農地 轉作光 電場   搭配 上游 補注 地下水   減緩 地層下陷   創造 地主   業者   政府   全民 與 綠能   五贏     前年 已達成 綠電供 應 全縣 民生 用電 階段 性 目標  </t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t xml:space="preserve">〔 記者 陳 彥廷 ／ 屏東 報導 〕 屏東縣 政府 於 東港   林邊   佳冬 枋寮 4 個 沿海 鄉鎮   劃定   嚴重 地層下陷區 光電計畫   專區   為確 保農民 耕作 權   不過   近來坊 間質 疑聲 浪漸 漲   環保局 強調   該區 計畫 發電量 為 800MW   百萬瓦     不會 無 限制 擴張   因此 至少 會 仍 3000 公頃 以上 農地 可供 農作     地面 型 光電場 成為 選戰 攻防 議題   屏東 因 沿海 嚴重 地層下陷區 為 全國 首個 縣府 核淮得 設光 電案場 專案   成 在野 黨攻 詰 對象   近期 坊 間 又 再 傳出 農民因 種電 失去 農保   老農 退場 又 留不住 青農及 蛇 鼠 窩 藏 副作用 等 爭議     屏縣 府 環保局 指出   這 4 鄉鎮過 去 因超 抽 地下水   曾列 為 嚴重 地層下陷區   現 仍屬 第 1   2 級 地下水 管制 區   且 海水 上溯 下   許多 土地 都 已 出現 鹽化   不少 已 是 不利 耕地 多年   因此 縣府 尊重 地主 利用 土地 意願 權益 前提 既有 電力 設施 併 網 上限 條件 下   限度 推動 光電 專區   預計 發電量 為 800MW     環保局 指出   部分 農地 轉作 太陽 光電 後   減少 農民 抽取 林邊 溪 下游 地下水 需求   並 搭配 上游 設置 大 潮州 人工湖 補注 地下水   減緩 地層下陷   達到 國土 復 育及 產業 永續 發展 目的   而 近年 同樣 大小 光電板 發電 效率 已較 八八 風災 後   養水 種電   到 近 2 倍   單 一片 就 可 發電達 400w   以 目前 併 網約 300MW 太陽光 電裝置 容量   使用 農地 比例 約 250 公頃 左右   未來 達 到 目標 單位 發電量 更大下   所 需面積 比例 一定 更 小   至少 會 3000 公頃 以上 農地 可供 農作 使用   另外   對 於 無力 管理 田間 工作   又 土地 鹽化 等 不利因素 無法 耕作 年 邁老農   則 可以 穩定 收入 過 退休 生活     至於 農保 問題   環保局 重申   農地 若 有意 願 出租 供 人 種電   一定 要 進行 變更 地目   但 這是 完全 基 於 地主 利用 土地 意願 權益   縣府 環保局 從 未 要求 廠商 提供 所謂   不利 耕作 同意 書   或 其他 網路 媒體 謠傳 不 平等 條約 相關 文件   先前 更 製 作 地主 注意 事項 手冊 Q &amp; A 圖卡   公告 於 縣府 綠辦 官網   讓 地主 了解 相關 權利 與 義務   只要 民眾 對 合約 疑問   均 可 撥 打 專線 電話詢 問綠能 專案 推動辦 公室   針對 部分 地區 爭議 案件   未 取得 居民 同意 之前   縣府 已 要求 業者 停止 施工     蛇鼠 患 問題   縣府 環保局 長 顏幸 苑則 認為   作物 收成 期間 食物 充沛 易 引鼠   鳥禽 覓 食   但 太陽能 案場 並無食源   應非屬 引鼠 主因   縣府 要求 專案 輔導業者 維護 周遭 環境 整潔   至於 選址 不當   縣府 重申   屏東縣 綠能 推動 政策 以   專案 專區 計畫       土地 複 合式 利用   兩大 策略 為主   專案 為 限度 使用 相對 不 適合 耕種 土地 發展 綠能   專案 專區 外 鄉鎮 優先 鼓勵 結合 既有 設施 與 光電   複 合 利用   方式     屏東縣 環保局 表示   民眾 對 於 光電 發展 與 環境 保護 議題 逐漸 重視   縣府 尊重 私有 地主 處置 自家 土地 財產   以及 業者 依法 申請 案件 權利   惟審查 過程將 審慎 關注 山坡地   耕作 農地   歷史 遺跡   生態 保育 或 重要 觀 光景 點聯絡 道路 沿線 等 議題   並 要求 廠商 提出 因應 作為   以 避免 衍生 爭議性 問題   兼顧 開發 合理性 及維護 本縣 農民 耕作 權益  </t>
+          <t xml:space="preserve">屏東 是 光電場 熱區 之一   正 上演 光電板 與 農民 搶 地爭 奪戰   光電業者 挨家 挨戶 以 誘人 租金 勸 說 地主 租地 種電   租地 種蓮霧 果農 只能 忍痛 看著 心血 被毀   斬斷 兒子 想 當青農 接班 願望   青農 自嘲 說   政府 寧可 把 地租 給業者 種電   不給 老 農一畝 田維生   青年 若當   漂鳥   回農村   肯定 變走 投無路   落翅仔         五十六 歲 鄭明偉 林邊   佳冬 鄉 租下 三座 蓮霧園   他 說   兩座 花 了 十多年 整理   收成 正漸 入 佳境   地主 竟 收回 種電   他 只能 忍痛 放棄   由 於 種蓮霧 要 手把手 長 期培養 技術   正在 念農校 兒子 雖 有心 接手   但 他 勸 兒子 算了   最好 另謀 出路                             農民控 國產署   為 賺 更 多 租金     屏東 沿海 不少 國有 財產 署名 下 新生 地   被 農 民用 於 種田   六十三 歲 楊寶秀 枋寮 寮 段種 芭樂   無奈說   種芭樂近 四十年   也繳 用地 補償 金給 國產署   一直 相安 無事   近年 數度 送件 申請 合法 承租 都 被 拒絕   後 來 光電業者 芭樂園 貼 告示 已 承租 種電   要 農民 及早 搬離   國產 署則 回覆 因 地層下陷 不利 耕作   要 轉作光 電場       六十多 歲 呂姓 老農 靠 這片 三分 地 蓮霧 園維生   他 說   國產署 明知 老農靠 種蓮霧 養家   寧可租 給光 電業者 賺 更 多   如果 沒地 可種     我 不但 要 吃 土   連農保 都 沒 了         面對 農民 控訴   國產署 南區 分署 屏東 辦 公室 指出   光電業者 依法 種電   並願意 取得 承租人 或 使用 人 同意 書 後 清理 地上 物   占用 者 繳 使用 補償 金   但 他們 本 就 沒 合法 使用 權       林邊   佳冬 枋寮   蓮霧 之 鄉   美名   四十八 歲 陳 呈祥 八八 風災後回 鄉 接手 父親 蓮霧園   他 感嘆   近年 光電大舉 入侵   正 侵蝕 果農 維 繫 傳 統 產 業 所 努力       他 說   蓮霧 老農因 子女 無意 接手   只好 租地 給光 電商   果園 地主 刻意 抬高 租金 逼退 承租 農   一塊 塊 果園 被 光電場 取代   包圍   整體 產量 正持續 下降   衝擊 採收   包裝   運銷 等 產業 鏈   未來 工人 更難 找   材料 更貴   務農條件 就 更 差       農地 租金 上漲   加速 產業 衰退     陳 呈祥 說   蓮霧 產業 衰退 人口老化   缺工 等 有關   雖 不能 全歸責 光電   但 確實 造成 農地 租金 上漲 問題   間接 加速 產業 衰退   政府 對 這些 衝突視 若 無睹   苦果 只 由 農民吞       枋寮 農會 總幹事 鄭晏昕   林邊 農會 總幹事 黃 金順 都 慨嘆   原盼 農電能 共生   如今 衝突 嚴重   地 驕傲 半世 紀的 蓮霧 產業   正因 光電 面臨 式微 危機       黃 金順 說   光電場 租金 一分 地四萬元   承租 農民頂 多出 得起 一萬元   相差 四倍   到 處 都 聽 到 地 主要 改 種電   年 輕人 想 返 鄉務農   無 低 租金 農地 可種     蓮霧 故鄉   金字招牌 正在 褪色       台大 農經 碩士 張靜玉 是 枋寮 蓮霧 農   眼看 鄰近 農民 被 光電 搶 地   忿忿不平   直指 當年 農委會 主委 蘇嘉全 還推 漂鳥 計畫   要 青年 返鄉務農   現在 連地 都 租 不到     這 不是 迫遷 青農去 都市 討 生活   漂鳥 回農村   恐怕 走 投無路 變 落翅仔    </t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -1587,7 +1587,7 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -1627,7 +1627,7 @@
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
@@ -1637,77 +1637,77 @@
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t xml:space="preserve">台北市 松山區 慶城街 一處 新建 工地 旁   昨天 晚間 發生 路面 塌陷 意外   經過 將近 20 小時 搶 救   工地 崩塌 範圍 已 完成 回填   今天下午 開始 灌漿 工地 外圍 塌陷 路面   初步 研判   疑似 是 新建 工程 拆除 建 地 既有 地下 建築 結構 時   挖到 不連續 弱面   才 導致 導溝 崩塌   台北市 松山區 慶城街 新建 工地 23 日 晚間 發 生地 層 坍陷 意外   經過 約 18 小時 緊急 搶 救   工地 外圍 崩塌 範圍終 於 展開 回填 作業   從制 高點 俯瞰 更 清楚   混 泥土 車來 回 進出 灌漿 沒 停過   因為 這一崩   不僅 人行道 嚴重 下陷   路邊 車格 消失 一大半   當時 還有 4 輛汽車 差點 被 吞噬   附近 住戶 直言     好 意外   真的 很 意外   文華飯 店 當初 蓋 時候 這麼 近   沒 發生過 問題     精華 地段 豪宅 新建 案出 現大 坍塌   讓 附近 居民 全都 嚇壞   畢竟 這長 約 4 公尺   寬約 30 公尺   深度 達到 1.5 公尺 坍陷 範圍 實在 不小   而且 建案 甚至 才 正 準備 施作 連續 壁   基礎 地基 都 還沒大規 模開 挖   竟然 就 前置 導溝 作業發 生意 外   初步 研判   坍塌 原因 跟 建地 原先 存在 地下室 結構 脫 不了 關 係   原來 這回 要 建立 深導溝   越過 既有 結構 時   卻 不慎 碰到 既存 不 連續面   才 會 釀禍   台北市 土木 技師 公會 理事 長 莊均緯 指出     破除 既有 連續 壁 跟 外牆   那個 地方 有個 不 連續面   原有 地下室 這個 部分   外牆 它 推擠 進來 變位   就 把 原來 深導溝 側壁壓 變形 之 後   就 產生 這樣 崩塌 現象     台北 市長 蔣萬安週 六 上午 二度 到 現場 勘查   向 居民 保證   周邊 住宅 暫無 安全 疑慮     西側   南側   北側 目前 比 對 監測 數值 是 正常   而且 都 沒 地面 塌陷 以及 鄰房 傾斜 狀況     建管處 則緊 急 開罰 18 萬   並 勒令停工   後 續 就 待 道路 回填   並由 透地雷達 確認 周邊 無 安全 疑慮   就 可 恢 復 通車   還給 居民 安全 環境  </t>
+          <t xml:space="preserve">〔 記者 陳 奕 劭 ／ 台北 報導 〕 台北市 松山區 慶城街 興安街 交叉路口 一處 工地   昨晚   23 日   發生 地基 塌陷   工地 旁有 4 輛停 路邊 停車格 轎車   車身 隨著 地基 塌陷 呈 70 度 傾斜   幸好 無人 傷亡   對此   台北市 前 市長 柯文 哲今 早   24 日   受訪 表示   台北市 是 地層下陷 警示 區   這是 本來 就 問題     台北市 松山區 慶城街 興安街 交叉路口 一處 工地 昨晚 發生 地基 塌陷   而 柯文 哲 卸任 後 發生 好 幾起 地層下陷 事件   柯文 哲今 早 關渡 宮前 受訪 表示   台北市 本來 就是 地層下陷 警示 區   其實 去 工務局 網站 看 就 知道   地層下陷 警示 區有 好 幾個   台北 是 盆地   這是 本來 就 問題     媒體 詢問   地層下陷 是 建商 問題 或是 地質 需進 一步 檢查   柯文 哲回 應   他們 地圖 已經 相當 完整   高 危險區 要 能夠 事先 知道  </t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t xml:space="preserve">台北市 慶城街 一處 新建 工地 昨晚 發生 地層下陷 事故   對 於 台北市 接連 發生 地層下陷 事件   前 台北 市長   民眾 黨 主席 柯文 哲 今天 表示   台北市 本來 就是 地層下陷 潛勢區   台北市 政府 已經 把 地圖 得 很 完整   要 知道 高 危險區   並做 必要 措施       柯文 哲 表示   台北市 本來 就是 地層下陷 潛勢區   其實 只要 去 工務局 往 上查 一下   就 可以 看到 地層下陷 潛勢區 好 幾個   因為 這個 地方 本來 就是 盆地   所以 就 會 這個 問題   目前 台北市 地圖 已經 相當 完整   高 危險區 要 事先 知道   做出 必要 措施  </t>
+          <t xml:space="preserve">台北市 松山區 慶城街 一處 新建 工地 昨   23   天晚間 發生 地基 塌陷 意外   停 路旁 4 台車 受到 波及   人行道 路面 凹陷   北市 府 緊急 成立 指揮 中心 處理   台北 市長 蔣萬安今 早 二度 到 現場 視察 現況   被 問及 北市 議員 許淑華 爆出 年前 就 接獲 異常 通報   市府 無 因應   對此 他 表示 會 請 建管處 全面 清查   台北 慶城街 塌陷 案   截至 上午 11 點   已 回填 360 立方公尺   回填 高度 已近 安全 目標值 3 公尺   約 12 點 左右 就 會 完成 作業   而 比 對 相關 數據 檢測   目前 僅有 塌陷 處東側 超過 15 公分 裂痕   西 南北 側比 對 監測 數值 正常   都 沒 地面 塌陷   鄰房 傾斜 狀況   管線   路樹 等 一 併 檢查 處理   此次 台北市 政府 昨晚 慶城街 工地 塌陷 事發 後   緊急 成立 指揮 中心   開罰 18 萬並 勒令 停業   要求 工作 灌漿 回填   確保 安全   這也 是 蔣萬安任 二度 建案 塌陷 發生   此次 處理 速度 較 上次 更 快   蔣萬安強 調   每 一次 事件 發生 都 會 一次 檢視   只要 機制 完善   每個 人員落 實運作   其實 反應 就 會 快速 確實   確保 各項 安全   讓 一切 恢 復 正常   不過 外界 質疑   相比 日前 雙北惡 臭案   市府 被質 疑動作 慢半拍   蔣萬安 回應   往後相關 機制 調整 完善   確 保人 員透過 機制 系統 運作   其實 各項 反應 就 能 即刻 因應   後 續 處理 就 會 到位   至於 許淑華 透露 年前 就 接獲 異常 通報   且 未來 可以 跟 外審 單位   大地   工程   結構 技師 等 一起 監工   對此 蔣萬安 表示   異常 通報   會 請 建管處 全面 清查     另外 此次 第一 時間 邀 請 四大 工會   技師   結構   大地   建築師 工會 參 與   謝 謝里長 到 現場 協助 各項 監測   這 部份 第一 時間 都 溝通 聯 繫  </t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t xml:space="preserve">台北市 松山區 慶城街 一處 新建 工地 昨   23   天晚間 發生 地基 塌陷 意外   停 路旁 4 台車 受到 波及   人行道 路面 凹陷   北市 府 緊急 成立 指揮 中心 處理   台北 市長 蔣萬安今 早 二度 到 現場 視察 現況   被 問及 北市 議員 許淑華 爆出 年前 就 接獲 異常 通報   市府 無 因應   對此 他 表示 會 請 建管處 全面 清查   台北 慶城街 塌陷 案   截至 上午 11 點   已 回填 360 立方公尺   回填 高度 已近 安全 目標值 3 公尺   約 12 點 左右 就 會 完成 作業   而 比 對 相關 數據 檢測   目前 僅有 塌陷 處東側 超過 15 公分 裂痕   西 南北 側比 對 監測 數值 正常   都 沒 地面 塌陷   鄰房 傾斜 狀況   管線   路樹 等 一 併 檢查 處理   此次 台北市 政府 昨晚 慶城街 工地 塌陷 事發 後   緊急 成立 指揮 中心   開罰 18 萬並 勒令 停業   要求 工作 灌漿 回填   確保 安全   這也 是 蔣萬安任 二度 建案 塌陷 發生   此次 處理 速度 較 上次 更 快   蔣萬安強 調   每 一次 事件 發生 都 會 一次 檢視   只要 機制 完善   每個 人員落 實運作   其實 反應 就 會 快速 確實   確保 各項 安全   讓 一切 恢 復 正常   不過 外界 質疑   相比 日前 雙北惡 臭案   市府 被質 疑動作 慢半拍   蔣萬安 回應   往後相關 機制 調整 完善   確 保人 員透過 機制 系統 運作   其實 各項 反應 就 能 即刻 因應   後 續 處理 就 會 到位   至於 許淑華 透露 年前 就 接獲 異常 通報   且 未來 可以 跟 外審 單位   大地   工程   結構 技師 等 一起 監工   對此 蔣萬安 表示   異常 通報   會 請 建管處 全面 清查     另外 此次 第一 時間 邀 請 四大 工會   技師   結構   大地   建築師 工會 參 與   謝 謝里長 到 現場 協助 各項 監測   這 部份 第一 時間 都 溝通 聯 繫  </t>
+          <t xml:space="preserve">台北市 慶城街   興安街 交叉口 昨   23   天晚間 突發生 工地 地基 塌陷 問題   連帶 週邊 停 路旁 汽車   人行道 傾斜 下陷   北市 府 緊急 下令 回填   經過 連夜 灌漿   截至 今   24   早 7 點 左右   已經 灌漿 250 方   初估 中午 12 點可 完成   另外 針對業者 開罰 18 萬並 勒令停工   據 了解   新建 工地 尚未 開挖   只是 導溝   疑似 因內部 支撐力 不夠   造成 導溝 外壁 下陷   所幸 無人 傷亡   而 除了 導溝 回填 外   北市 府 表示 外側 坍塌 處   為 預防樹木 傾倒   且 灌漿 回填 後 樹木無法 存活   故將 4 棵 黑板 樹鋸斷   此外   北市 府 開罰 業者 18 萬   並 勒令停工   而 雖然 目前 沒有 漏水 情況   但 接下 來 自來 水處 將持續 監測   早上 會 進場 透地雷達 檢測   並確 認管線 排水 溝 是否 破壞 處理 方式   待 基地 內側 灌漿 完成 初 凝 後   即 進行 道路 回填   北市 府 透露   今早 沒 再 塌陷 情況   監測 資料 今天 比 對 完成 後 公布  </t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t xml:space="preserve">〔 記者 陳 奕 劭 ／ 台北 報導 〕 台北市 松山區 慶城街 興安街 交叉路口 一處 工地   昨晚   23 日   發生 地基 塌陷   工地 旁有 4 輛停 路邊 停車格 轎車   車身 隨著 地基 塌陷 呈 70 度 傾斜   幸好 無人 傷亡   對此   台北市 前 市長 柯文 哲今 早   24 日   受訪 表示   台北市 是 地層下陷 警示 區   這是 本來 就 問題     台北市 松山區 慶城街 興安街 交叉路口 一處 工地 昨晚 發生 地基 塌陷   而 柯文 哲 卸任 後 發生 好 幾起 地層下陷 事件   柯文 哲今 早 關渡 宮前 受訪 表示   台北市 本來 就是 地層下陷 警示 區   其實 去 工務局 網站 看 就 知道   地層下陷 警示 區有 好 幾個   台北 是 盆地   這是 本來 就 問題     媒體 詢問   地層下陷 是 建商 問題 或是 地質 需進 一步 檢查   柯文 哲回 應   他們 地圖 已經 相當 完整   高 危險區 要 能夠 事先 知道  </t>
+          <t xml:space="preserve">台北市 松山區 慶城街   興安街 一處 新建 工地   昨   23   天晚間 發生 地基 塌陷 意外   造成 停 路旁 四台 車 受到 波及   人行道 路面 呈現 V 字型 凹陷   面積 約 4 公尺 長   30 公尺 寬   深度 約 1.5 公尺   所幸 週邊 建築物 沒有 危險   相關 單位 連夜 現場 進行 回填 作業   不過 工地 遭罰 18 萬 勒令停工   事發 原因 尚待 調查   慶城街 新建 工地 地基 下陷   路面 坍塌   人行道   工程 圍籬 都 明顯 下陷   路旁 停車格 消失 一大半   當時 路邊 4 輛汽車 遭殃 歪斜   建商 連夜 回填 灌漿   避免 塌陷 擴大   據 了解   該 處興 建工 地原 是 要 蓋 豪宅 大樓   原先 工地 上 地下 三層 地下室 建物   疑似 拆除 建物 後   地下室 進行 導溝 作業 時候   內部導 溝支 撐力 不足 才 發生 坍塌 意外   所幸 工地 尚未 進行 大規模 開 挖   沒 再 釀 更 大 事故   此次 路面 坍塌 面積長 約 4 公尺   寬約 30 公尺   深度 1.5 公尺   目前 週邊 建築物 沒有 相關 安危   而 北市 建管處 勘查 後   昨天 深夜 確定 裁罰 18 萬   並 勒令 回填 穩定 後 停工   待 確保 工地 安全   業者   建商 提出 復工 審查   才 會 進行後續 作業   至於 事發 原因 仍待 調查  </t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t xml:space="preserve">台北市 慶城街   興安街 交叉口 昨   23   天晚間 突發生 工地 地基 塌陷 問題   連帶 週邊 停 路旁 汽車   人行道 傾斜 下陷   北市 府 緊急 下令 回填   經過 連夜 灌漿   截至 今   24   早 7 點 左右   已經 灌漿 250 方   初估 中午 12 點可 完成   另外 針對業者 開罰 18 萬並 勒令停工   據 了解   新建 工地 尚未 開挖   只是 導溝   疑似 因內部 支撐力 不夠   造成 導溝 外壁 下陷   所幸 無人 傷亡   而 除了 導溝 回填 外   北市 府 表示 外側 坍塌 處   為 預防樹木 傾倒   且 灌漿 回填 後 樹木無法 存活   故將 4 棵 黑板 樹鋸斷   此外   北市 府 開罰 業者 18 萬   並 勒令停工   而 雖然 目前 沒有 漏水 情況   但 接下 來 自來 水處 將持續 監測   早上 會 進場 透地雷達 檢測   並確 認管線 排水 溝 是否 破壞 處理 方式   待 基地 內側 灌漿 完成 初 凝 後   即 進行 道路 回填   北市 府 透露   今早 沒 再 塌陷 情況   監測 資料 今天 比 對 完成 後 公布  </t>
+          <t xml:space="preserve">台北 松山區 慶城街 昨   23   天晚間 發生 地層下陷   身為 前 台北 市長   民眾 黨 主席 柯文 哲今 早 挑戰 一日 北高   被 問到 卸任 後 北市 兩度 發生 工地 地層下陷   他 表示 台北市 是 盆地   本來 就是 地層下陷 檢視區   認為 高 危險區 要 能夠 事先 知道   並做 必要措施   柯文 哲 今天 一大早 6 點多   從 台北 關渡 宮出 發挑戰 一日 北高   面對慶 城街 昨晚 發生 地層下陷   他 認為 台北市 本來 就是 地層下陷 檢視區   工務 局網 站上 可以 看到 好 幾個 區域   且 北市 本來 就是 盆地   所以 本來 就 這個 問題   至於 問題 出 誰 身上   柯文 哲認 為   本來 地質 就 應該 多 注意   北市 地路 已經 相當 完整   高 危險區 要 能夠 事先 知道   必要措施 防範  </t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t xml:space="preserve">台北 松山區 慶城街 昨   23   天晚間 發生 地層下陷   身為 前 台北 市長   民眾 黨 主席 柯文 哲今 早 挑戰 一日 北高   被 問到 卸任 後 北市 兩度 發生 工地 地層下陷   他 表示 台北市 是 盆地   本來 就是 地層下陷 檢視區   認為 高 危險區 要 能夠 事先 知道   並做 必要措施   柯文 哲 今天 一大早 6 點多   從 台北 關渡 宮出 發挑戰 一日 北高   面對慶 城街 昨晚 發生 地層下陷   他 認為 台北市 本來 就是 地層下陷 檢視區   工務 局網 站上 可以 看到 好 幾個 區域   且 北市 本來 就是 盆地   所以 本來 就 這個 問題   至於 問題 出 誰 身上   柯文 哲認 為   本來 地質 就 應該 多 注意   北市 地路 已經 相當 完整   高 危險區 要 能夠 事先 知道   必要措施 防範  </t>
+          <t xml:space="preserve">台北市 松山區 慶城街 一處 新建 工地 旁   昨天 晚間 發生 路面 塌陷 意外   經過 將近 20 小時 搶 救   工地 崩塌 範圍 已 完成 回填   今天下午 開始 灌漿 工地 外圍 塌陷 路面   初步 研判   疑似 是 新建 工程 拆除 建 地 既有 地下 建築 結構 時   挖到 不連續 弱面   才 導致 導溝 崩塌   台北市 松山區 慶城街 新建 工地 23 日 晚間 發 生地 層 坍陷 意外   經過 約 18 小時 緊急 搶 救   工地 外圍 崩塌 範圍終 於 展開 回填 作業   從制 高點 俯瞰 更 清楚   混 泥土 車來 回 進出 灌漿 沒 停過   因為 這一崩   不僅 人行道 嚴重 下陷   路邊 車格 消失 一大半   當時 還有 4 輛汽車 差點 被 吞噬   附近 住戶 直言     好 意外   真的 很 意外   文華飯 店 當初 蓋 時候 這麼 近   沒 發生過 問題     精華 地段 豪宅 新建 案出 現大 坍塌   讓 附近 居民 全都 嚇壞   畢竟 這長 約 4 公尺   寬約 30 公尺   深度 達到 1.5 公尺 坍陷 範圍 實在 不小   而且 建案 甚至 才 正 準備 施作 連續 壁   基礎 地基 都 還沒大規 模開 挖   竟然 就 前置 導溝 作業發 生意 外   初步 研判   坍塌 原因 跟 建地 原先 存在 地下室 結構 脫 不了 關 係   原來 這回 要 建立 深導溝   越過 既有 結構 時   卻 不慎 碰到 既存 不 連續面   才 會 釀禍   台北市 土木 技師 公會 理事 長 莊均緯 指出     破除 既有 連續 壁 跟 外牆   那個 地方 有個 不 連續面   原有 地下室 這個 部分   外牆 它 推擠 進來 變位   就 把 原來 深導溝 側壁壓 變形 之 後   就 產生 這樣 崩塌 現象     台北 市長 蔣萬安週 六 上午 二度 到 現場 勘查   向 居民 保證   周邊 住宅 暫無 安全 疑慮     西側   南側   北側 目前 比 對 監測 數值 是 正常   而且 都 沒 地面 塌陷 以及 鄰房 傾斜 狀況     建管處 則緊 急 開罰 18 萬   並 勒令停工   後 續 就 待 道路 回填   並由 透地雷達 確認 周邊 無 安全 疑慮   就 可 恢 復 通車   還給 居民 安全 環境  </t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t xml:space="preserve">台北市 松山區 慶城街   興安街 一處 新建 工地   昨   23   天晚間 發生 地基 塌陷 意外   造成 停 路旁 四台 車 受到 波及   人行道 路面 呈現 V 字型 凹陷   面積 約 4 公尺 長   30 公尺 寬   深度 約 1.5 公尺   所幸 週邊 建築物 沒有 危險   相關 單位 連夜 現場 進行 回填 作業   不過 工地 遭罰 18 萬 勒令停工   事發 原因 尚待 調查   慶城街 新建 工地 地基 下陷   路面 坍塌   人行道   工程 圍籬 都 明顯 下陷   路旁 停車格 消失 一大半   當時 路邊 4 輛汽車 遭殃 歪斜   建商 連夜 回填 灌漿   避免 塌陷 擴大   據 了解   該 處興 建工 地原 是 要 蓋 豪宅 大樓   原先 工地 上 地下 三層 地下室 建物   疑似 拆除 建物 後   地下室 進行 導溝 作業 時候   內部導 溝支 撐力 不足 才 發生 坍塌 意外   所幸 工地 尚未 進行 大規模 開 挖   沒 再 釀 更 大 事故   此次 路面 坍塌 面積長 約 4 公尺   寬約 30 公尺   深度 1.5 公尺   目前 週邊 建築物 沒有 相關 安危   而 北市 建管處 勘查 後   昨天 深夜 確定 裁罰 18 萬   並 勒令 回填 穩定 後 停工   待 確保 工地 安全   業者   建商 提出 復工 審查   才 會 進行後續 作業   至於 事發 原因 仍待 調查  </t>
+          <t xml:space="preserve">台北市 慶城街 一處 新建 工地 昨晚 發生 地層下陷 事故   對 於 台北市 接連 發生 地層下陷 事件   前 台北 市長   民眾 黨 主席 柯文 哲 今天 表示   台北市 本來 就是 地層下陷 潛勢區   台北市 政府 已經 把 地圖 得 很 完整   要 知道 高 危險區   並做 必要 措施       柯文 哲 表示   台北市 本來 就是 地層下陷 潛勢區   其實 只要 去 工務局 往 上查 一下   就 可以 看到 地層下陷 潛勢區 好 幾個   因為 這個 地方 本來 就是 盆地   所以 就 會 這個 問題   目前 台北市 地圖 已經 相當 完整   高 危險區 要 事先 知道   做出 必要 措施  </t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
@@ -1717,7 +1717,7 @@
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
@@ -1727,7 +1727,7 @@
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
@@ -1737,7 +1737,7 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
@@ -1757,87 +1757,87 @@
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t xml:space="preserve">新北 萬里 加頭 溫泉 2 月份 被 遊客 發現   不僅 燈管   溫度 顯示氣 等等 設備 問題   更 地層下陷   因此 趕緊 請 公所 找人 檢修   目前 已經 緊急 封閉   確認 沒有 安全 疑慮   才 會 再度 開放     浴池 整塊 磁磚 脫落   地磚 不平   甚至 還 有些 地層下陷   看起 來 相當 老舊   這裡 是 新北 萬里 加頭 溫泉   從 日據 時代起   就 受到 不少 民眾 喜愛   許多人 泡 完湯   都 覺得 放 鬆 筋骨     不過 2 月份 卻 被 發現   不僅 燈管   溫度 顯示器   一些 溫泉 管線 設備 問題 外   還有 地層下陷 跡象   鐵鋁罐 放在 地上   都 會 不 自主   滾向 一邊   加上 後 方 就是 溫泉 露頭   要是 坍方 相當 危險   萬里區 長 黃 雱 勉     技師 建議 我們   要 專業 技師 公會 去   針對 結構物 下陷 狀況   去 監測   評估後續 是不是 可以 用   液壓 灌漿 部分 改善       地質 人員 透過 地雷 達 偵測 結果 發現   確實 男女 湯內 地底   大量 孔隙   造成 土壤 流失   目前 公所 已經   緊急 封閉 浴室   以民眾 安全 為 第一 考量   盡快 修建       封面 圖 ／ 東森新聞  </t>
+          <t>新北市 萬里 區加 投溫泉 公共 浴室 疑似 地層下陷 現象   為確 保泡湯 安全   目前 已 封閉 修繕 中     公所 提供     中央社 記者 王鴻國 傳真   113 年 3 月 26 日</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>萬里區 公 所以 訊息 說明   萬里 區加 投溫泉 公共 浴室 於 日據 時代 建造   歷史 悠久   屬 於 海底 溫泉   為 當地 居民 從小到 大泡 湯空間     區 公所 表示   因 2 月底 有民眾 反應 浴室 燈管   溫度 顯示器 不亮 等 問題   於 是 委 託 廠商 勘查 後 發現   疑似 地層下陷 現象   為確 保泡湯 安全   已 封閉 浴室     區長 黃 雱 勉 表示   為 瞭解 確切 原因   找出 有效 改善 方法   將邀 請 專業 技師 進行 檢查 評估   以商 討後續 改善 辦法   期望 安全 前提 下   儘 早 恢 復 提供 民眾 泡 湯空間   提醒 民眾 封閉 期間 勿 擅自 進入 使用   以維護 自身 安全     萬里區 公所 主任 秘書 許明富 向 中央社 記者 表示   當地過 去 地層下陷   並 完成 改善 多年   未影響 溫泉 供給 溫度   加投 溫泉 公共 浴室 經找 技師 以 透地雷達 探測 後   男女 湯室 地下 發現 土壤 流失 現象   未來將 進行 修繕 改善   並確 認無 危險 之 虞   才 會 再行 開放 供民眾 使用     編輯   林恕暉   1130326</t>
+          <t>新北市 萬里 區加 投溫泉 公共 浴室 疑似 地層下陷 現象   造成 浴池 受損   壁磚 脫落   未來將 進行 修繕 改善   確認 無 危險 之 虞   才 會 再行 開放 供民眾 使用     公所 提供     中央社 記者 王鴻國 傳真   113 年 3 月 26 日</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>新北市 萬里區 公所 表示   有民眾 日前 反應加 投溫泉 公共 浴室 燈管   溫度 顯示器 不亮 等 問題   委 託 廠商 勘查 後 發現   疑似 地層下陷 現象   圖為 建物 出現 裂縫     公所 提供     中央社 記者 王鴻國 傳真   113 年 3 月 26 日</t>
+          <t>新北市 萬里   加投 溫泉   公共 浴室   算是 古 蹟 了   它 是 日據 時期 就 蓋 好   而且 到現 很多 人   喜歡 來 這裡 泡湯   不過 上個 月 開始   這裡 出現 大大小小 問題   浴池 磁磚 掉落   水泥柱 裂痕   地面 嚴重 傾斜   因此 現在 浴池 已經 暫時 封閉 了   等到 廠 商都 修繕 完畢   確認 安全 都 沒 問題   才 會 再度 開放       鏡新聞 已 上架 86 台   若無法 收看   請 洽詢 當地系 統台     鏡新聞 APP   iOS 👉 https   reurl . cc kqyqML   鏡新聞 APP   Android 👉 https   reurl . cc Ay2y63   有話 鏡來講 YT 👉 https   reurl . cc A4DjQj   少年 新聞 週記 YT 👉 https   reurl . cc K4DeN9</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t xml:space="preserve">新北市 萬 里加 投溫泉 公共 浴室 歷史 悠久   吸引 許多人 前來 泡湯   不過   今年 2 月   有民眾 反應 溫泉 設備 出 問題   沒 想到 廠商 進場 維修 後   發現 浴池 磁磚 掉落   水泥柱 充滿 裂痕   地面 嚴重 傾斜 等 狀況   更 仔細 勘查 下   竟然 地層下陷 現象   地質 檢測 人員 檢查   原來 湯室 地底 大量 孔隙   造成 土壤 流失   目前 封閉 整修     鋁罐 放在 地上 一路 滾 不停   不 只 地面 嚴重 傾斜   浴池 還有 一 大片 磁磚 脫落   水泥柱 充滿 裂痕   原來 這處 溫泉 發生 地層下陷     新北市 萬 里加 投溫泉 公共 浴室 日治時 代興建   歷史 相當 悠久   水質 相當 不錯   吸引 許多人 前來 泡湯     不過 今年 2 月 開始   就 泡 湯遊客 反應   燈管   溫度 顯示器 溫泉 管線 設備 問題   區 公所 派 人 前往 了解 狀況   由廠 商進場 維修   發現 不 只是 設備 故障   還有 磁磚 脫落   地磚 不 平等 狀況   仔細 勘查 下 發現 地層下陷 現象   公所 從 4 號開始 封閉 浴室   趕緊 找 專業 技師 到場 檢查   男女 湯室 地底 大量 孔隙   造成 土壤 流失   懷疑 可能 跟 一旁 溫泉 露頭 有關 係     大鵬里長 李建才     露頭 我 不敢 說絕 對 沒 有關 係   因為 這個 是 相通 東西   地底下 看不到   以 目前 整個 狀況 來講 話   下陷 狀況 速度 應該 不是 很 急速   這是 很多年 類似 有點 掏空 感覺       溫泉 從 溫泉 露頭 自然 湧出   抽到 蓄水池 後   流入 浴池   可能 連帶 影響 地基 被 掏空     萬里區 長 黃 雱 勉     技師 建議 我們 要 專業 技師 公會   針對 結構物 下陷 狀況 去 監測   再 去 評 估後續 是不是 可以 用液 壓 灌漿 部分 改善   還是 可能 要大動 作去 做後續 改建   這個 部分 後 續 可能 會 需要 比較 多 費用       公所 強 調 儘 快 修建 完成   提供 民眾 安全 舒適 泡 湯空間  </t>
+          <t xml:space="preserve">〔 記者 俞肇福 ／ 新北 報導 〕 日治 時代 建造 新北市 萬里 區加 投溫泉 公共 浴室   因 係 屬免 費泡湯   不但 金山 萬里 當地民眾 喜愛   就連 基隆 人 搭車 專程 前來 免費 泡湯   因 日前 發現 疑似 地層下陷   萬里區 公所 立即 封閉 浴室   並邀 請 專業 技師 與 工程 廠商 勘查   將於 完成 改善 並確 認無 危險   才 會 再行 開放     新北市 議員 周雅玲 表示   接 獲當 地民眾 反映   加投 溫泉 公共 浴室 屋頂 漏水   排水 不良   牆有 裂縫 等 事宜   廠商 到場 會勘 後 發現   懷疑 是 地層下陷   為確 保民 眾泡湯 安全   自 3 月 4 日 起先 封閉 浴室   經技師 以 透地雷達 探測 後   男女 湯室 地底下 土壤 流失 現象   公所 再度 發起 現勘   商討後續 改善 辦法     周雅玲 指出   萬 里加 投溫泉 公共 浴室 10 多年 前 曾 經修繕   當時 就 曾 經有 出動 透地雷達 探測   這次 透地雷達 探測   與 當年 比較 發現 問題 較 為 嚴重   建議 應該 邀請 土木 技師 一 併 會勘   包含 溫泉 主管 機關 經濟 發展局   水利局 邀請 來   對 於 周邊 溫泉開 發應 予以 總量 管制   以免 加投 溫泉 公共 浴室 慘遭 池魚 之殃     萬里區 區長 黃 雱 勉 表示   加投 溫泉 公共 浴室 經專業 技師 檢視   發現 下陷 致建築物 傾斜 情形   為 瞭解 確切 原因   找出 有效 改善 方法   公所 將再 請 新北市 土木 技師 公會 等 相關 專家 進行 專業 檢查 評估   期望 確保 安全 無虞 前提 下   儘 早 恢 復 提供 民眾 泡 湯空間   呼籲   加投 溫泉 公共 浴室 封閉 期間   民眾 切勿 擅 闖 翻越 圍籬 進入 使用   以維護 自身 安全  </t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t xml:space="preserve">〔 記者 俞肇福 ／ 新北 報導 〕 日治 時代 建造 新北市 萬里 區加 投溫泉 公共 浴室   因 係 屬免 費泡湯   不但 金山 萬里 當地民眾 喜愛   就連 基隆 人 搭車 專程 前來 免費 泡湯   因 日前 發現 疑似 地層下陷   萬里區 公所 立即 封閉 浴室   並邀 請 專業 技師 與 工程 廠商 勘查   將於 完成 改善 並確 認無 危險   才 會 再行 開放     新北市 議員 周雅玲 表示   接 獲當 地民眾 反映   加投 溫泉 公共 浴室 屋頂 漏水   排水 不良   牆有 裂縫 等 事宜   廠商 到場 會勘 後 發現   懷疑 是 地層下陷   為確 保民 眾泡湯 安全   自 3 月 4 日 起先 封閉 浴室   經技師 以 透地雷達 探測 後   男女 湯室 地底下 土壤 流失 現象   公所 再度 發起 現勘   商討後續 改善 辦法     周雅玲 指出   萬 里加 投溫泉 公共 浴室 10 多年 前 曾 經修繕   當時 就 曾 經有 出動 透地雷達 探測   這次 透地雷達 探測   與 當年 比較 發現 問題 較 為 嚴重   建議 應該 邀請 土木 技師 一 併 會勘   包含 溫泉 主管 機關 經濟 發展局   水利局 邀請 來   對 於 周邊 溫泉開 發應 予以 總量 管制   以免 加投 溫泉 公共 浴室 慘遭 池魚 之殃     萬里區 區長 黃 雱 勉 表示   加投 溫泉 公共 浴室 經專業 技師 檢視   發現 下陷 致建築物 傾斜 情形   為 瞭解 確切 原因   找出 有效 改善 方法   公所 將再 請 新北市 土木 技師 公會 等 相關 專家 進行 專業 檢查 評估   期望 確保 安全 無虞 前提 下   儘 早 恢 復 提供 民眾 泡 湯空間   呼籲   加投 溫泉 公共 浴室 封閉 期間   民眾 切勿 擅 闖 翻越 圍籬 進入 使用   以維護 自身 安全  </t>
+          <t xml:space="preserve">新北市 萬 里加 投溫泉 公共 浴室 歷史 悠久   吸引 許多人 前來 泡湯   不過   今年 2 月   有民眾 反應 溫泉 設備 出 問題   沒 想到 廠商 進場 維修 後   發現 浴池 磁磚 掉落   水泥柱 充滿 裂痕   地面 嚴重 傾斜 等 狀況   更 仔細 勘查 下   竟然 地層下陷 現象   地質 檢測 人員 檢查   原來 湯室 地底 大量 孔隙   造成 土壤 流失   目前 封閉 整修     鋁罐 放在 地上 一路 滾 不停   不 只 地面 嚴重 傾斜   浴池 還有 一 大片 磁磚 脫落   水泥柱 充滿 裂痕   原來 這處 溫泉 發生 地層下陷     新北市 萬 里加 投溫泉 公共 浴室 日治時 代興建   歷史 相當 悠久   水質 相當 不錯   吸引 許多人 前來 泡湯     不過 今年 2 月 開始   就 泡 湯遊客 反應   燈管   溫度 顯示器 溫泉 管線 設備 問題   區 公所 派 人 前往 了解 狀況   由廠 商進場 維修   發現 不 只是 設備 故障   還有 磁磚 脫落   地磚 不 平等 狀況   仔細 勘查 下 發現 地層下陷 現象   公所 從 4 號開始 封閉 浴室   趕緊 找 專業 技師 到場 檢查   男女 湯室 地底 大量 孔隙   造成 土壤 流失   懷疑 可能 跟 一旁 溫泉 露頭 有關 係     大鵬里長 李建才     露頭 我 不敢 說絕 對 沒 有關 係   因為 這個 是 相通 東西   地底下 看不到   以 目前 整個 狀況 來講 話   下陷 狀況 速度 應該 不是 很 急速   這是 很多年 類似 有點 掏空 感覺       溫泉 從 溫泉 露頭 自然 湧出   抽到 蓄水池 後   流入 浴池   可能 連帶 影響 地基 被 掏空     萬里區 長 黃 雱 勉     技師 建議 我們 要 專業 技師 公會   針對 結構物 下陷 狀況 去 監測   再 去 評 估後續 是不是 可以 用液 壓 灌漿 部分 改善   還是 可能 要大動 作去 做後續 改建   這個 部分 後 續 可能 會 需要 比較 多 費用       公所 強 調 儘 快 修建 完成   提供 民眾 安全 舒適 泡 湯空間  </t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>新北市 萬里   加投 溫泉   公共 浴室   算是 古 蹟 了   它 是 日據 時期 就 蓋 好   而且 到現 很多 人   喜歡 來 這裡 泡湯   不過 上個 月 開始   這裡 出現 大大小小 問題   浴池 磁磚 掉落   水泥柱 裂痕   地面 嚴重 傾斜   因此 現在 浴池 已經 暫時 封閉 了   等到 廠 商都 修繕 完畢   確認 安全 都 沒 問題   才 會 再度 開放       鏡新聞 已 上架 86 台   若無法 收看   請 洽詢 當地系 統台     鏡新聞 APP   iOS 👉 https   reurl . cc kqyqML   鏡新聞 APP   Android 👉 https   reurl . cc Ay2y63   有話 鏡來講 YT 👉 https   reurl . cc A4DjQj   少年 新聞 週記 YT 👉 https   reurl . cc K4DeN9</t>
+          <t>新北市 萬里區 公所 表示   有民眾 日前 反應加 投溫泉 公共 浴室 燈管   溫度 顯示器 不亮 等 問題   委 託 廠商 勘查 後 發現   疑似 地層下陷 現象   圖為 建物 出現 裂縫     公所 提供     中央社 記者 王鴻國 傳真   113 年 3 月 26 日</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>新北市 萬里 區加 投溫泉 公共 浴室 疑似 地層下陷 現象   為確 保泡湯 安全   目前 已 封閉 修繕 中     公所 提供     中央社 記者 王鴻國 傳真   113 年 3 月 26 日</t>
+          <t>萬里區 公 所以 訊息 說明   萬里 區加 投溫泉 公共 浴室 於 日據 時代 建造   歷史 悠久   屬 於 海底 溫泉   為 當地 居民 從小到 大泡 湯空間     區 公所 表示   因 2 月底 有民眾 反應 浴室 燈管   溫度 顯示器 不亮 等 問題   於 是 委 託 廠商 勘查 後 發現   疑似 地層下陷 現象   為確 保泡湯 安全   已 封閉 浴室     區長 黃 雱 勉 表示   為 瞭解 確切 原因   找出 有效 改善 方法   將邀 請 專業 技師 進行 檢查 評估   以商 討後續 改善 辦法   期望 安全 前提 下   儘 早 恢 復 提供 民眾 泡 湯空間   提醒 民眾 封閉 期間 勿 擅自 進入 使用   以維護 自身 安全     萬里區 公所 主任 秘書 許明富 向 中央社 記者 表示   當地過 去 地層下陷   並 完成 改善 多年   未影響 溫泉 供給 溫度   加投 溫泉 公共 浴室 經找 技師 以 透地雷達 探測 後   男女 湯室 地下 發現 土壤 流失 現象   未來將 進行 修繕 改善   並確 認無 危險 之 虞   才 會 再行 開放 供民眾 使用     編輯   林恕暉   1130326</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>新北市 萬里 區加 投溫泉 公共 浴室 疑似 地層下陷 現象   造成 浴池 受損   壁磚 脫落   未來將 進行 修繕 改善   確認 無 危險 之 虞   才 會 再行 開放 供民眾 使用     公所 提供     中央社 記者 王鴻國 傳真   113 年 3 月 26 日</t>
+          <t xml:space="preserve">新北 萬里 加頭 溫泉 2 月份 被 遊客 發現   不僅 燈管   溫度 顯示氣 等等 設備 問題   更 地層下陷   因此 趕緊 請 公所 找人 檢修   目前 已經 緊急 封閉   確認 沒有 安全 疑慮   才 會 再度 開放     浴池 整塊 磁磚 脫落   地磚 不平   甚至 還 有些 地層下陷   看起 來 相當 老舊   這裡 是 新北 萬里 加頭 溫泉   從 日據 時代起   就 受到 不少 民眾 喜愛   許多人 泡 完湯   都 覺得 放 鬆 筋骨     不過 2 月份 卻 被 發現   不僅 燈管   溫度 顯示器   一些 溫泉 管線 設備 問題 外   還有 地層下陷 跡象   鐵鋁罐 放在 地上   都 會 不 自主   滾向 一邊   加上 後 方 就是 溫泉 露頭   要是 坍方 相當 危險   萬里區 長 黃 雱 勉     技師 建議 我們   要 專業 技師 公會 去   針對 結構物 下陷 狀況   去 監測   評估後續 是不是 可以 用   液壓 灌漿 部分 改善       地質 人員 透過 地雷 達 偵測 結果 發現   確實 男女 湯內 地底   大量 孔隙   造成 土壤 流失   目前 公所 已經   緊急 封閉 浴室   以民眾 安全 為 第一 考量   盡快 修建       封面 圖 ／ 東森新聞  </t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
@@ -1847,7 +1847,7 @@
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
@@ -1897,7 +1897,7 @@
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>-1</v>
+        <v>12</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
@@ -1917,7 +1917,7 @@
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>24</v>
+        <v>-1</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
@@ -1947,7 +1947,7 @@
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
@@ -1957,7 +1957,7 @@
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
@@ -1977,7 +1977,7 @@
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
@@ -1987,7 +1987,7 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
@@ -1997,7 +1997,7 @@
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
@@ -2007,7 +2007,7 @@
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
@@ -2017,7 +2017,7 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
@@ -2027,7 +2027,7 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
@@ -2047,7 +2047,7 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
@@ -2057,7 +2057,7 @@
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
@@ -2067,7 +2067,7 @@
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -2077,7 +2077,7 @@
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
@@ -2087,7 +2087,7 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -2097,7 +2097,7 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
@@ -2107,7 +2107,7 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
@@ -2117,7 +2117,7 @@
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
@@ -2127,7 +2127,7 @@
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
@@ -2137,7 +2137,7 @@
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
@@ -2147,7 +2147,7 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
@@ -2167,7 +2167,7 @@
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
@@ -2177,7 +2177,7 @@
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
@@ -2187,7 +2187,7 @@
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
@@ -2197,11 +2197,101 @@
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
           <t xml:space="preserve">科技 大亨 馬 斯克   Elon   Musk   今天   5 19   抵達 印尼 峇里島   將與 印尼 總統 佐科威   Joko   Widodo   一起 參加 星鏈   Starlink   網路 服務 啟用   印尼 將是 東南亞 第三 個 使用 星鏈 服務 國家   政府 希望 星鏈 能夠 提高 各島嶼 網路 普及 度   這是 印尼 一個 月 迎接 第 3 名 科技 企業 執行長   此前 蘋果   微軟 執行長 都 已來訪     綜合 路透社 與 美聯社 報導   太空 科技 公司 SpaceX 執行長 馬 斯克 今天 搭乘 私人 飛機 抵達 印尼 峇里島 機場   印尼 首席 投資部長 盧胡特   Luhut   Binsar   Pandjaitan   機場 迎接   預計 兩人 將會 討論 一些 重要 合作   包含 星鏈 服務 啟動   馬 斯克 還會 簽署 一項 協助 印尼 加強 衛生 與 教育 單位 聯絡 互通 合約     盧胡特 表示   馬 斯克 今天 稍晚 將和 印尼 總統 佐科威 一起 峇里島 首府 登巴薩   Denpasar   社區 衛生 中心 一起 啟動 星鏈   盧胡特 說   衛生 機構 啟動 這項 服務   呼應 星鏈   提供 平價 高速 網路   宗旨   尤其 是 網路 收訊 不佳 或過 於 偏遠 地區     印尼 是 個 群島 國家   約 1.7 萬座 島嶼   橫跨 3 個 時區   人口 超過 2.7 億   盧胡特 說   印尼 偏鄉 需要 星鏈 來 拓展 高速 網路   尤其 是 要 用 來 解決 衛生   教育 海事 單位 問題     印尼 通訊 部長 布迪   Budi   Arie   Setiadi   上週 表示   星鏈 已經 獲得 印尼 營運許 可   布迪 強調   星鏈 低 軌衛星 可以 讓 網路 擴及 目前 印尼 通訊 商無法 到 達 地區     據報   位 於 印尼 婆羅洲   Borneo   新 首都 努山 塔拉   Nusantara   本月 將先 試用 星鏈   8 月 正式 上線   印尼 正準備 遷都 努山 塔拉   因為 受 海平面 上升 與 地層下陷 影響   預計 目前 首都 雅加 達 大部分 地區將 2050 年 被淹 沒     印尼 將是 東南亞 第三 個 使用 星鏈 服務 國家   馬 來 西亞 去年 已核 發許 可證 給營 運星鏈 SpaceX 公司   菲律賓 一家 公司 則是 2022 年 與 SpaceX 簽約 合作     馬 斯克訪 印尼 前   蘋果 公司 執行長 庫克   Tim   Cook   4 月 17 與 印尼 總統佐科 威會面   並 表示 會將 印尼 產能 納入 考慮   兩周 後   微軟 執行長 納 德拉   Satya   Nadella   同月 30 日訪 印尼   承諾 未來 4 年 印尼 投資 17 億 美元   強化 印尼 新雲端 運算 與 人工智慧 基礎 設施     馬 斯克 此次 訪 峇里島   將參加 第十 屆 世界 水論壇   World   Water   Forum     研討 全球 水資源 衛生 挑戰  </t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>0</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">[ 周刊 王 CTWANT ]   花蓮市 名店   歪 歪歪 甜點     南京 街 店面 竟 被後方 建案   廣朋   建設 公司 以修繕 名義 直接 將廁 所 拆除   業者 忍無可忍 報警 處理   而廣朋 於 建設 新大樓 過程 當中 造成 鄰損 不 只 這一樁   一名 A 房屋 剛好位 基地 旁邊   房屋 早已 因 地層下陷 而 硬生生 斷成 兩截   而廣朋 不但 試圖將 相關 損害 歸咎 於 地震   且 只 買 了 一個 大 水桶 讓 住 戶接 漏水   讓 住戶 完全 無法 接受     A 帶著 本刊 記者 實際 走 進屋   儘 管 該 棟 房屋 為 老舊 3 層 透天   但 屋內 深度 相當 深   穿越 車庫 進入 客廳 後 可以 明顯 感覺 地層 已 下陷   腳下 磁磚 碎裂   屋主 已 鋪 上 軟 墊   避免 踩 上面 時 受傷     A 拿出 一顆 乒乓球 放在 地面 測試 屋內 地板 磁磚 水平   且 明顯 看見 本該 靜止 乒乓球 滾動   證明 地面 出現 傾斜   A 憤怒 表示     這些 損害 早 0403 大 地震 前 就 已經 發生   廣朋還 試圖 想要 將責任 全部 歸咎 地震 上       A 帶著 記者 穿越 客廳 進入 一樓後方 臥室   不但 明顯 感受 到 地面 傾斜   地上 更裂 出 一條 又 深 又 長 裂縫   一路 到 房屋 正後方   而後方 因 房屋 管線 受損 嚴重 已 無電力 照明   A 隨手 拿 起 一條 目測 至少 約 1 公尺 長 木棍   直接 插 進裂 開 縫 中   他 裂縫 中 攪動 木棍 表示     這裂 縫 寬度 至少 約 5 公分   而 這根 木棍 甚至 還沒 到底   跟 我 說 這叫 地震 造成       走上 2 樓   由 於 房屋 後 半段 傾斜   門框 早已 變形 無法 關上   管線 被 嚴重 破壞   不但 沒有 電力 照明   水還 從 四面八方 滴滴答答 滲出   A 說   這樣 到底 要 怎麼 住   而 廣朋所 事 就是   買 了 一個 大 水桶 要 我們 接 漏水       當地 主商里 里 長 廖大慶 5 月 22 日 帶 著 縣府 與 市公所 人員 前往 工地 會勘   廖大慶 比著 工地 一旁 柏油路 上 明顯 裂痕 與 民宅 地板 明顯 落差 表示     這 不是 地層下陷 是 什麼     廣朋 李姓 協理則 表示   柏油路 裂痕 已有 補過   但 主要 應是 3   40 噸 重機具 每天 這裡 進出 所導致   里長 吐 槽 表示     不要 跟 我 說 是 重機具   那為 什麼 只有 工地 這 一段 出現 裂痕 下陷   工地 前 後 柏油路 都 沒 裂開     場面 一度 相當 火爆     22 日 會勘 住 戶 對 建商 一片 罵聲 中 暫時 落幕   花蓮縣 議員 吳東 昇 居中 協調   廣朋 初步 承諾會 先將 裂開 下陷 馬 路 進行 修繕   以維護 公共安全   至於 與 住 戶 所 造成 鄰損 等 狀況   雙方遲 遲無法 達 成共識   因此 相關 損害 修 復 恐怕 還有 得 吵     廣朋總 公司 位 於 台北 市長 安東路   其 於 104 上 敘述 自稱 成立 20 年來 擁有 專業 建築 團隊   除 專注 北市 市中心 精華區 興建 精 緻 住宅   同時 將建築 領域 開發 至 花蓮市   台南 與 高雄   同時 更是 ViVi   PARK 停車 品牌 經營者     但 廣朋在 2017 年 時 與 台灣 知名 視障 慢跑 者     台灣 阿甘   之稱 張文彥 發生 租屋 糾紛   張文彥 向 廣朋租 店面 開設 視障 健康 按摩 養生會館   但 廣朋 卻 將停 車場 以金 店面 名義 承租 給張 文彥   並 要求 提前 解約   甚至 將 店面 大門 以鐵片 封死   搬 2 塊 巨石 擋住 大門   被 批 手段 惡劣   而前 台北市 議員 黃 向 羣 曾 被 周刊 踢 爆   其為 北捷 萬大線   捷七聯 開案   地主 拒絕 加入 聯合 開發 一事   以 優先 投資權   開發 獲利 超過 13 億元 吸引 地主 找廣朋 合作   以此 收取 6500 萬元 顧 問費   造成 地主 200 坪 土地 被 納入 聯開   市價 5 億 多元 土地 僅能 拿 回 1 億餘元     對此   本刊 兩度致 電向位 北市 廣朋總 公司 詢問   該 公司 接線 人員 表示 對 此事 不 了解   並說 公司 沒 有人 可 代表 對外 說明   就 將電話 掛斷   不再 回應  </t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>16</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">江慶賢 指出   近一個 月 立信 街   信街   自強 街 附近 住戶   不斷 反映 水壓 不足   很多 里民因 為 抽 不到 水   馬 達 都 燒壞 了   他 向 自來 水 公司 反映   水 公司 一開始 堅持 水壓 供水 都 正常   最後才 說 水管 破裂   今天 要來 修理     今   5   日 早上 江慶賢還 沒 等到 水 公司 工程 人員   就 接到 里民通報   指立 中 六街 出現 天坑   他 跑 到 現場   見 到 一部 工程 車右後輪 將馬路 壓出 一個 洞   怪手 正在 協助 工程 車脫 困   幸好 沒人 傷亡   但馬路 破洞 裡的 水源 源不斷 湧出   地層下陷 情形 似乎 很 嚴重   他將 要求 自來 水 公司 全力 補救     自來 水 公司 回應 表示   一開始 以 為 只是 漏水   後 來 才 發現 立中 六街 下方 還有 一處 直徑 10 公分 自來 水管 線 破裂   當下 已 立即 派遣 工班 到場 處理   針對 住戶 抽水 馬 達 燒壞   將會 研議 是否 進行 相關 賠償  </t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>5</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">台灣 西南 沿海 地區 為候 鳥 主要 度冬棲息 地   為 了 守護 於 此 休憩 黑面 琵鷺   水鳥 與 候鳥   台灣 環境 資訊 協會   簡稱 環資   嘉時 航運 股份 有限公司   簡稱 嘉時 航運   攜手 合作 生態 工作 假期   於 5 月 27 日至 嘉義 布袋 濕地   執行 棲地 植樹 活動   讓候 鳥 過境 休憩 時   樹林 保護下 安心 成長   更 期盼 長 期 努力 下   成為 全球 生物 多樣 性 後 盾     嘉義 布袋 擁有 廣闊 濕地 多樣 鳥類 棲息 地   以豐富 生態 資源 特色 環境 聞名   這裡 每年 冬季 都 會 迎來 一批 特別 客人   是 全球 關注 物種 — — 黑面 琵鷺   從 1989 年 全球 紀錄 288 隻   到 2024 年 共 6988 隻   數量 變化 一直 受到 國際 鳥類 保護 組織 密切 追 蹤     天氣剛 好 遇到 5 月 梅雨季   各地 受 鋒面 與 氣流 影響   很 幸運 受到 天公 伯伯 賞臉   讓 雲層 遮住 炙熱 太陽   陰涼 天氣 下 順利 進行     志工 雙手 從 平常 使用 電腦 與 滑鼠   換成 圓鍬 鏟子   互相 協助 挖出 半 公尺 深 與 寬 土穴   倒入 蚵 殼 抵擋 鹽氣   細心 覆土種 下 適合 濱 海生 長 木麻黃   黃 槿 大葉欖仁 樹苗   總共種 下 40 棵 樹   廣闊 環境 中 工作   志工 臉 因 挖掘 動作 變得 通紅   休補充 水分 時   抬頭望 就 能 看 見 波光粼粼 濕地 中   鳥類 生活 覓食 畫面   相信 大家 不僅 是 為 黑面 琵鷺 保護 出力   更是 為 全球 生物 多樣 性 維護 做出 貢獻     本次 環資 活動 總籌乙雯 說     相信 經過 今天 棲地 行動   我們 都 更 貼 近 腳下 這片 土地   了解 生態 保育 重要性       嘉義 擁有 著 美好 生態 棲地外   面臨 著 多重 環境 挑戰   工作 完成 後   志工 搭 上 遊覽車 移動 前往 白水 湖壽島   走訪 2020 年   消失 情人 節   電影 壯闊 海景 美麗夕陽 背 後   沒有 說 出 國土 消失   地層下陷   影響 生態 系統 健康 現況     嘉義 因優越 水質 地勢 條件   使養 蚵 產業 蓬勃 發展   外海 密密麻麻 竹棚   近岸 漂浮 白色 保麗龍   垂 吊式 養殖 道路 上 暫放 成山 蚵 殼   從 眼前 景色 就 能 了解 牡蠣 不同 養殖 方式   志工 走 隔 開陸 地 與 海 堤防 上   右手 邊是 海   左手 邊是 滯洪池   蔡 福昌 老師 說     現在 大家 腳下 堤防 近幾年 修建 加高   如果 不 這麼   陸 地上 坐路 掌潭村 就 會 淹 沒 危險     吹 著涼爽 海風   遠方 風力 發電機 運轉 著   退潮 時 沿著 海水 與 紅磚 被 海 水淹 沒 痕跡   水泥 路上 長 滿蘚類   可以 走向 外 海沙 島的 方向   感受 濱海 滄桑 與 失落     志工文 函用 望眼 鏡發現 高蹺 鴴   又名 長 腳 鷸 身影   一雙長 紅腿 淺水 地上 行走   欣賞 之餘 用 手機 連接 著望 遠鏡 鏡頭   拍下 它們 拍 翅 美姿     來 到 嘉義 不 只有 食 蚵   嘉時 航運 志工 不僅付 諸行動   守護 遠道 來 台 黑面 琵鷺 與候 鳥棲地   還相約 下次 再 到 布袋 濕地   樹下 乘涼   欣賞候 鳥 安心 棲息 美好 畫面   成為 生物 多樣 性守護者  </t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>0</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t xml:space="preserve">此外   住 戶質 疑公會 鑑定 專業   表示 重災戶 房子 傾斜 倒塌   不 就是 基泰 跟 技師 做出 來   安全 無虞證 明書     才 引起 這場 重大 公安   住戶 質疑現 鑑定   結構 安全     誰 能 保證 是 真的 安全     陳 怡君 提到   住戶 表示   對 於 下陷 地層   家中 磁磚 脫落   地 磚裂 掉   門窗 鐵門壞 掉   家中 漏水 水管 破裂   天花板 掉落 等   賠償 1.2 倍 相當 沒誠意   除了 財產 損失   多處 損鄰 造成 生活 不便   家中 隨時 磁磚 脫落 精神 折磨   還有 地震 來時 不安   這些 精神 賠償     陳 怡君 說   這是 損鄰戶 第一次 公部門 主導 下 所 召開 調解會議   基泰 應正視 損鄰戶 心聲   針對 賠償 金額   陳 怡 君主 張應 提高 為 1.5 倍   或主動 至 損鄰戶 家中 估價除 結構 之外 損失   增列 至 賠償 金額 中   才 是 該 賠償 氣度     對此   據   自由 時報   報導   台北市 建管處 表示   為 促進 基泰 與 受 損戶 協調 和解 效率   都 發局 主動 本月 6 日 於 大直 國小辦 理代為 協調 會議   針對 會議 中受 損戶 提出 修繕 賠償 金額 不足 等 訴求   已 請 基泰 建設 收集 受 損戶 所 提相 關意 見後並 妥為 處理   促進 建損 雙方 和解 進度  </t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>24</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t xml:space="preserve">原來 同一 個 新能源 市場   同時 這麼 多 幫人 市場 上 探索   開發     圖片 來源 ／ Pixabay  </t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>5</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">記者 林意筑 ／ 台中 報導   台中港 西碼頭 附近   今   11   日 上午 一度 傳出 碼頭 破堤 消息   透過 現場 畫面 可見   一部 重型 機具 因 不明 原因 深陷 海砂 中   一旁 海水 幾乎 快 淹過   引發民眾 恐慌   不過 稍早 警方 緊急 澄清   由 於 該 起 工程 作業 本身 就 海平面 以下   因此 下 挖 管線 時   因 海水 壓力 導致 機具 下沉   並非 地層下陷 引起 海水倒灌     據悉   台中港 西碼頭 中油 區 近日 正在 進行 建造 冷凝 設備 工程 作業   但 今日 上午 一度 傳出   大型 機具 因 不明 原因 深陷 海砂 中   造成 恐慌     對此   台中港 務西 碼頭 中隊 長 賴逸丰 表示   由 於 該 起 工程 作業   挖 埋 管線   部分 本身 就 海平面 以下   而 下 挖 管線 時 因 海水 壓力 差而導致 機具 下沉   並非 地層下陷 引起 海水倒灌   預計 今日 下午 抽完 海水 後 即可 繼續 作業   現場 無人員 受傷   無 相關 設備 建物 損壞  </t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>17</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">近期 能源 公司 元長 鄉 瓦 磘 村 建 設 太 陽 光 電 場   卻 場址 設 村莊 中心   讓 當地 居民 人心惶惶   今 ( 11 ) 日 瓦 磘 反光 電 自救 會 前往 雲林縣 議會   向 縣長 張麗善 遞交陳情 書   盼光 電廠 商 另 尋他 地   不要 將光 電場 設置 於 瓦 磘 村 中   張麗善 除 親手 接下 陳 情書   表示 會 站 鄉親 立場   保護 大家 居住 環境   呼籲台 電應 考量 民眾 意見 本權責 妥處     張麗善 表示   地方 政府 跟 中央政府 都 各自 權責   公務人員 需要 配合 行政 程序   目前 法令 規定   若 是 建地 就 可以 百分之百 種電   雲林縣 農地 很多   地層下陷   易 淹水   不利 耕作 土地   已經 被 中央 核定 為 合法 種電 範圍     張麗善 再次 強調   三不三要     不 希望 農地 一直 種電   破壞 農地 未來 發展 跟 價值   認為 光電業者 聚落 裡 種電   已影響 鄉親 生活 起居 跟 品質   能 感同身受 鄉親 不安 焦慮   會 透過 各種 協調 溝通   保障 地 鄉親 權益     建設 處長 李俊 興 表示   本案 屬於鄉 村區 乙種 建築 用地   業者 依法 向 縣府 提出 申請   公部門 亦 依法行政 核發 同意 文件   去年 9 月 接 獲民眾 陳 情 後   立即 協調 業者 應 與 當地 居民 持續 溝通   業者 表示同意 先行 暫停 施工  </t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>17</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t xml:space="preserve">陳 安邦 等 表示   種電 可以 村外   村內 緊鄰 民宅   不要 說 危害   打 開家門   窗戶 看到 就是 太陽 能板   叫 8   90 歲 老人 情 何以堪   尤其 庄內 種電 作為   請問 哪個 村 可以 接受   所以 村民 大團 結堅 決展 現反 對 到底 決心   任何 回饋 都 不用 說   打死 都 反 對 庄內 種電   任何 法律 問題 他 一個 人承擔   甚至 為 了 爭取 縣長 張麗善 村民 主持公道   特別 今天 前來 向 張縣 長 陳 情   唯一 要求 光場 業者 退出 瓦 磘 村     縣長 張麗善 接下 陳 情書 後 指出   地方 政府 跟 中央政府 都 各自 權責   公務人員 需要 配合 行政 程序   目前 法令 規定   若 是 建地 就 可以 百分之百 種電   雲林縣 農地 很多   地層下陷   易 淹水   不利 耕作 土地   已經 被 中央 核定 為 合法 種電 範圍   為 了 保護 我們 農地   特別 提出 三不三要   就是 不 希望 農地 上面 一直 種電   破壞 農地 未來 發展 跟 價值   光電業者 聚落 裡面 種電   已經 影響 鄉親 生活 起居 跟 品質   大家 不安 焦慮 我們 都 能 感同身受   縣府 透過 各種 協調 溝通   希望 能 保障 地 鄉親 權益  </t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>-1</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">張信 哲杜拜 站 演唱 會 原定 2 月 登場   後 來 撞 上 極端 氣候 出現 冰雹   淹水 災害   因而 延期 至 端午 假期 6 月 9 日舉行   他 笑 說     很 開心   差點 變成 不是 第一 個     透露 目前 已經 很多 歌手   陸續 安排 開唱 計畫   原本 很 擔心 阿拉伯 國家 演出 會 很多 限制   像是 有些 景點 不能 比 出 特定 手勢   演唱 會太過 喧鬧   後 來 才 發現 他們 對 外國人 很 禮遇   很 支持 娛樂 活動     第一次 得知 邀請 時   張信哲 心想     真的假 啦   有人 要 聽     過往 都 只有 杜拜 轉機 經驗   從 未 入境 過旅遊 他 說     他們 來 邀 請 時 就 說   以中 東來 說 這邊 是 華人 最 多 地方   30 萬人     杜拜位 處國際 航班 交通 樞紐   因此 有來 自 歐洲   俄羅斯 華人 歌迷   特地 飛來 欣賞 演唱 會   因為 天災 延期 開唱   歌迷 們 沒 太 多 抱怨 問題   把 票 留著 就 為 了 等到 正式 演出 這 一天 朝聖     首次 前進 沙漠 開唱   張信哲 歌喉 完全 沒有 受 影響     還好   場館 冷氣 很足   我 提前 4 天來   杜拜   調時 差     本來 就 沒 計畫 要 衝場 次 演出   1 週 1 場已 是 最大 限度     未來式   巡演 開唱 6 年   亞洲 站 預計 至 2024 年底 結束   前進 海外 開唱   他 最 想 攻 佔 場館 是 英國倫敦 皇家 阿爾伯特 音樂廳   Royal   Albert   Hall       張信 哲新 專輯 已經 籌備 中   下半年 會釋 出 更 多 新歌   台北 小 巨蛋   高雄 巨蛋 演唱 會   則要 排到 2025 年 才能 開唱     第一 個 要 搶 時間   現在 場館 太難 搶 了     記者 提議 大 巨蛋 開唱   張信哲 卻 謙虛回     大 巨蛋 周董   周杰倫   都 還排 不到   哪 還輪 到 我   等 別人 有空 給我用   我 再 用 就 好       歌神 張學友 因為 身體 不適   日前 取消 台北 站 演唱 會   張信哲 關注 此事     好 害怕   我 吃 增強 免疫力 的藥   醫生開     即將 前進 海拔 2000 多 公尺 青海 西寧站 開唱   張信哲 提到   前輩   薛之謙唱 到 吸氧 氣   私下 還嚇 他     一定 不要 亂動   不要 突然 爆衝    </t>
         </is>
       </c>
     </row>

</xml_diff>